<commit_message>
First release of Part III
</commit_message>
<xml_diff>
--- a/Shared/polys.xlsx
+++ b/Shared/polys.xlsx
@@ -3159,7 +3159,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3319,7 +3319,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3359,7 +3359,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3559,7 +3559,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3679,7 +3679,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3919,7 +3919,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3959,7 +3959,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4119,7 +4119,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4319,7 +4319,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4519,7 +4519,7 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4599,7 +4599,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4839,7 +4839,7 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4999,7 +4999,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5119,7 +5119,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="J120" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5319,7 +5319,7 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5399,7 +5399,7 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5479,7 +5479,7 @@
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5559,7 +5559,7 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5679,7 +5679,7 @@
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5719,7 +5719,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5799,7 +5799,7 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5839,7 +5839,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5959,7 +5959,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6039,7 +6039,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6119,7 +6119,7 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6199,7 +6199,7 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6279,7 +6279,7 @@
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6319,7 +6319,7 @@
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6399,7 +6399,7 @@
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6439,7 +6439,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6519,7 +6519,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6559,7 +6559,7 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6599,7 +6599,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6639,7 +6639,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6679,7 +6679,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6719,7 +6719,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6759,7 +6759,7 @@
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6799,7 +6799,7 @@
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6839,7 +6839,7 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6879,7 +6879,7 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6959,7 +6959,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6999,7 +6999,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7079,7 +7079,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7119,7 +7119,7 @@
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7159,7 +7159,7 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7199,7 +7199,7 @@
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7279,7 +7279,7 @@
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7319,7 +7319,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7359,7 +7359,7 @@
       </c>
       <c r="J173" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7399,7 +7399,7 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7439,7 +7439,7 @@
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7479,7 +7479,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved some cases from Part I to Part II
</commit_message>
<xml_diff>
--- a/Shared/polys.xlsx
+++ b/Shared/polys.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J214"/>
+  <dimension ref="A1:J221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -6738,28 +6738,28 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>2.2.b_b</t>
+          <t>2.2.a_c</t>
         </is>
       </c>
       <c r="F158" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G158" t="n">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>[4, 6, 13, 26, 14, 63, 116, 274, 589, 966, 2050, 3935, 8168]</t>
+          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>[0, 6, 21, 42, 30, 63, 84, 210, 525, 966, 2178, 4191, 8424]</t>
+          <t>[0, 10, 9, 18, 30, 55, 168, 306, 513, 1150, 2178, 3855, 7956]</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6774,27 +6774,27 @@
         <v>2</v>
       </c>
       <c r="D159" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>2.2.a_c</t>
+          <t>2.2.b_b</t>
         </is>
       </c>
       <c r="F159" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G159" t="n">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
+          <t>[4, 6, 13, 26, 14, 63, 116, 274, 589, 966, 2050, 3935, 8168]</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>[0, 2, 9, 2, 30, 23, 168, 242, 513, 1022, 2178, 3599, 7956]</t>
+          <t>[0, 6, 21, 42, 30, 63, 84, 210, 525, 966, 2178, 4191, 8424]</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
@@ -6814,32 +6814,32 @@
         <v>2</v>
       </c>
       <c r="D160" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F160" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G160" t="n">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>[0, 2, 12, 26, 0, 56, 126, 290, 516, 902, 1716, 3884, 8190]</t>
+          <t>[1, 5, 25, 25, 41, 65, 113, 225, 385, 1025, 2113, 4609, 8321]</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6858,23 +6858,23 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>2.2.b_d</t>
+          <t>2.2.a_c</t>
         </is>
       </c>
       <c r="F161" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G161" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
+          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>[0, 2, 12, 14, 30, 44, 189, 302, 534, 1172, 2079, 4136, 8073]</t>
+          <t>[0, 2, 9, 2, 30, 23, 168, 242, 513, 1022, 2178, 3599, 7956]</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
@@ -6898,28 +6898,28 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>2.2.c_c</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F162" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G162" t="n">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>[0, 2, 15, 26, 30, 47, 126, 194, 375, 1082, 2046, 4703, 8502]</t>
+          <t>[0, 2, 12, 26, 0, 56, 126, 290, 516, 902, 1716, 3884, 8190]</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6931,35 +6931,35 @@
         <v>3</v>
       </c>
       <c r="C163" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D163" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>3.2.ab_c_a</t>
+          <t>2.2.b_d</t>
         </is>
       </c>
       <c r="F163" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G163" t="n">
-        <v>200</v>
+        <v>55</v>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>[2, 8, 14, 32, 22, 56, 142, 224, 518, 968, 1982, 4400, 8374]</t>
+          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
+          <t>[0, 2, 12, 14, 30, 44, 189, 302, 534, 1172, 2079, 4136, 8073]</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6971,35 +6971,35 @@
         <v>3</v>
       </c>
       <c r="C164" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D164" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>3.2.a_b_a</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F164" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G164" t="n">
-        <v>144</v>
+        <v>13</v>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>[3, 7, 9, 23, 33, 103, 129, 191, 513, 967, 2049, 3983, 8193]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>[0, 0, 9, 0, 30, 93, 168, 144, 513, 900, 2178, 3741, 7956]</t>
+          <t>[0, 2, 15, 26, 30, 47, 126, 194, 375, 1082, 2046, 4703, 8502]</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7018,28 +7018,28 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>3.2.a_b_d</t>
+          <t>3.2.ab_c_a</t>
         </is>
       </c>
       <c r="F165" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G165" t="n">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>[3, 7, 18, 23, 18, 76, 108, 263, 459, 1012, 2247, 4172, 8310]</t>
+          <t>[2, 8, 14, 32, 22, 56, 142, 224, 518, 968, 1982, 4400, 8374]</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>[0, 0, 18, 0, 15, 66, 147, 216, 459, 945, 2376, 3930, 8073]</t>
+          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7058,23 +7058,23 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>3.2.b_b_b</t>
+          <t>3.2.a_b_a</t>
         </is>
       </c>
       <c r="F166" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G166" t="n">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>[4, 6, 10, 22, 44, 90, 74, 254, 496, 966, 2050, 4198, 8636]</t>
+          <t>[3, 7, 9, 23, 33, 103, 129, 191, 513, 967, 2049, 3983, 8193]</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 24, 30, 90, 42, 288, 462, 900, 1848, 3810, 8580]</t>
+          <t>[0, 0, 9, 0, 30, 93, 168, 144, 513, 900, 2178, 3741, 7956]</t>
         </is>
       </c>
       <c r="J166" t="inlineStr">
@@ -7098,23 +7098,23 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>3.2.b_b_e</t>
+          <t>3.2.a_b_d</t>
         </is>
       </c>
       <c r="F167" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G167" t="n">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>[4, 6, 19, 10, 44, 63, 116, 194, 523, 1146, 2116, 4063, 8012]</t>
+          <t>[3, 7, 18, 23, 18, 76, 108, 263, 459, 1012, 2247, 4172, 8310]</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>[0, 0, 21, 12, 30, 63, 84, 228, 489, 1080, 1914, 3675, 7956]</t>
+          <t>[0, 0, 18, 0, 15, 66, 147, 216, 459, 945, 2376, 3930, 8073]</t>
         </is>
       </c>
       <c r="J167" t="inlineStr">
@@ -7138,28 +7138,28 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>3.2.b_c_a</t>
+          <t>3.2.b_b_b</t>
         </is>
       </c>
       <c r="F168" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G168" t="n">
-        <v>200</v>
+        <v>108</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>[4, 8, 4, 32, 44, 56, 116, 224, 508, 968, 2116, 4400, 8012]</t>
+          <t>[4, 6, 10, 22, 44, 90, 74, 254, 496, 966, 2050, 4198, 8636]</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 32, 60, 24, 84, 96, 444, 840, 2244, 4400, 8268]</t>
+          <t>[0, 0, 12, 24, 30, 90, 42, 288, 462, 900, 1848, 3810, 8580]</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7178,23 +7178,23 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>3.2.b_c_b</t>
+          <t>3.2.b_b_e</t>
         </is>
       </c>
       <c r="F169" t="n">
         <v>21</v>
       </c>
       <c r="G169" t="n">
-        <v>189</v>
+        <v>63</v>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>[4, 8, 7, 28, 39, 71, 88, 220, 574, 943, 2138, 4375, 8051]</t>
+          <t>[4, 6, 19, 10, 44, 63, 116, 194, 523, 1146, 2116, 4063, 8012]</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 24, 45, 60, 105, 264, 669, 1065, 2145, 4368, 7800]</t>
+          <t>[0, 0, 21, 12, 30, 63, 84, 228, 489, 1080, 1914, 3675, 7956]</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
@@ -7218,28 +7218,28 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>3.2.b_c_e</t>
+          <t>3.2.b_c_a</t>
         </is>
       </c>
       <c r="F170" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G170" t="n">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>[4, 8, 16, 16, 24, 80, 88, 256, 520, 1168, 2072, 3808, 8168]</t>
+          <t>[4, 8, 4, 32, 44, 56, 116, 224, 508, 968, 2116, 4400, 8012]</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>[0, 0, 21, 12, 30, 69, 105, 300, 615, 1290, 2079, 3801, 7917]</t>
+          <t>[0, 0, 12, 32, 60, 24, 84, 96, 444, 840, 2244, 4400, 8268]</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7258,28 +7258,28 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>3.2.b_d_e</t>
+          <t>3.2.b_c_b</t>
         </is>
       </c>
       <c r="F171" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G171" t="n">
-        <v>243</v>
+        <v>189</v>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>[4, 10, 13, 18, 14, 79, 116, 242, 589, 1030, 2050, 3807, 8168]</t>
+          <t>[4, 8, 7, 28, 39, 71, 88, 220, 574, 943, 2138, 4375, 8051]</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>[0, 2, 21, 18, 30, 47, 84, 114, 525, 902, 2178, 3807, 8424]</t>
+          <t>[0, 0, 12, 24, 45, 60, 105, 264, 669, 1065, 2145, 4368, 7800]</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7298,28 +7298,28 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>3.2.b_e_e</t>
+          <t>3.2.b_c_d</t>
         </is>
       </c>
       <c r="F172" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G172" t="n">
-        <v>360</v>
+        <v>161</v>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>[4, 12, 10, 16, 14, 72, 158, 224, 550, 1032, 1918, 4144, 8246]</t>
+          <t>[4, 8, 13, 20, 29, 83, 74, 236, 562, 1103, 2116, 3887, 8363]</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>[0, 6, 12, 18, 0, 72, 126, 258, 516, 966, 1716, 3756, 8190]</t>
+          <t>[0, 0, 21, 20, 45, 51, 42, 108, 498, 975, 2244, 3887, 8619]</t>
         </is>
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7338,23 +7338,23 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>3.2.c_d_f</t>
+          <t>3.2.b_c_d</t>
         </is>
       </c>
       <c r="F173" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G173" t="n">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>[5, 7, 14, 15, 40, 52, 82, 311, 545, 1072, 1919, 4212, 7870]</t>
+          <t>[4, 8, 13, 20, 29, 83, 74, 236, 562, 1103, 2116, 3887, 8363]</t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>[1, 1, 16, 17, 26, 52, 50, 345, 511, 1006, 1717, 3824, 7814]</t>
+          <t>[0, 2, 15, 22, 15, 83, 42, 270, 528, 1037, 1914, 3499, 8307]</t>
         </is>
       </c>
       <c r="J173" t="inlineStr">
@@ -7378,28 +7378,28 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>3.2.c_e_h</t>
+          <t>3.2.b_c_e</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="G174" t="n">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>[5, 9, 14, 9, 25, 78, 103, 305, 518, 1029, 1853, 4158, 8611]</t>
+          <t>[4, 8, 16, 16, 24, 80, 88, 256, 520, 1168, 2072, 3808, 8168]</t>
         </is>
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>[1, 1, 22, 9, 41, 46, 71, 177, 454, 901, 1981, 4158, 8867]</t>
+          <t>[0, 0, 21, 12, 30, 69, 105, 300, 615, 1290, 2079, 3801, 7917]</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7418,23 +7418,23 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>3.2.c_e_h</t>
+          <t>3.2.b_d_e</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G175" t="n">
-        <v>152</v>
+        <v>243</v>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>[5, 9, 14, 9, 25, 78, 103, 305, 518, 1029, 1853, 4158, 8611]</t>
+          <t>[4, 10, 13, 18, 14, 79, 116, 242, 589, 1030, 2050, 3807, 8168]</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>[1, 3, 16, 11, 11, 78, 71, 339, 484, 963, 1651, 3770, 8555]</t>
+          <t>[0, 2, 21, 18, 30, 47, 84, 114, 525, 902, 2178, 3807, 8424]</t>
         </is>
       </c>
       <c r="J175" t="inlineStr">
@@ -7458,28 +7458,28 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>3.2.d_h_l</t>
+          <t>3.2.b_e_e</t>
         </is>
       </c>
       <c r="F176" t="n">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="G176" t="n">
-        <v>224</v>
+        <v>360</v>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>[6, 10, 6, 14, 26, 82, 118, 286, 474, 930, 2294, 4046, 7962]</t>
+          <t>[4, 12, 10, 16, 14, 72, 158, 224, 550, 1032, 1918, 4144, 8246]</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>[2, 2, 14, 14, 42, 50, 86, 158, 410, 802, 2422, 4046, 8218]</t>
+          <t>[0, 6, 12, 18, 0, 72, 126, 258, 516, 966, 1716, 3756, 8190]</t>
         </is>
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7491,30 +7491,30 @@
         <v>3</v>
       </c>
       <c r="C177" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D177" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>4.2.d_f_i_n</t>
+          <t>3.2.c_d_f</t>
         </is>
       </c>
       <c r="F177" t="n">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="G177" t="n">
-        <v>424</v>
+        <v>99</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>[6, 6, 15, 22, 21, 87, 97, 214, 510, 1151, 2118, 4123, 7793]</t>
+          <t>[5, 7, 14, 15, 40, 52, 82, 311, 545, 1072, 1919, 4212, 7870]</t>
         </is>
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>[0, 0, 18, 4, 20, 42, 42, 92, 540, 1090, 2068, 3814, 8008]</t>
+          <t>[1, 1, 16, 17, 26, 52, 50, 345, 511, 1006, 1717, 3824, 7814]</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
@@ -7531,35 +7531,35 @@
         <v>3</v>
       </c>
       <c r="C178" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D178" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>4.2.d_f_k_s</t>
+          <t>3.2.c_e_h</t>
         </is>
       </c>
       <c r="F178" t="n">
-        <v>117</v>
+        <v>38</v>
       </c>
       <c r="G178" t="n">
-        <v>351</v>
+        <v>152</v>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>[6, 6, 21, 18, 6, 63, 132, 306, 525, 966, 1986, 4191, 8040]</t>
+          <t>[5, 9, 14, 9, 25, 78, 103, 305, 518, 1029, 1853, 4158, 8611]</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>[0, 0, 18, 0, 0, 72, 126, 360, 549, 990, 1683, 4212, 8073]</t>
+          <t>[1, 1, 22, 9, 41, 46, 71, 177, 454, 901, 1981, 4158, 8867]</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7571,35 +7571,35 @@
         <v>3</v>
       </c>
       <c r="C179" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D179" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>4.2.e_j_q_z</t>
+          <t>3.2.c_e_h</t>
         </is>
       </c>
       <c r="F179" t="n">
-        <v>171</v>
+        <v>38</v>
       </c>
       <c r="G179" t="n">
-        <v>513</v>
+        <v>152</v>
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>[7, 7, 13, 19, 17, 85, 77, 291, 589, 1027, 1921, 3949, 8405]</t>
+          <t>[5, 9, 14, 9, 25, 78, 103, 305, 518, 1029, 1853, 4158, 8611]</t>
         </is>
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>[0, 0, 21, 12, 30, 75, 84, 180, 525, 960, 2178, 3963, 8424]</t>
+          <t>[1, 3, 16, 11, 11, 78, 71, 339, 484, 963, 1651, 3770, 8555]</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7611,30 +7611,30 @@
         <v>3</v>
       </c>
       <c r="C180" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D180" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>4.2.e_k_u_bg</t>
+          <t>3.2.d_h_l</t>
         </is>
       </c>
       <c r="F180" t="n">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="G180" t="n">
-        <v>585</v>
+        <v>224</v>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>[7, 9, 13, 9, 17, 81, 161, 225, 481, 1089, 1921, 4353, 7937]</t>
+          <t>[6, 10, 6, 14, 26, 82, 118, 286, 474, 930, 2294, 4046, 7962]</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>[0, 2, 21, 2, 30, 71, 168, 114, 417, 1022, 2178, 4367, 7956]</t>
+          <t>[2, 2, 14, 14, 42, 50, 86, 158, 410, 802, 2422, 4046, 8218]</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
@@ -7658,23 +7658,23 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>4.2.f_o_bc_bs</t>
+          <t>4.2.d_f_i_n</t>
         </is>
       </c>
       <c r="F181" t="n">
-        <v>260</v>
+        <v>106</v>
       </c>
       <c r="G181" t="n">
-        <v>520</v>
+        <v>424</v>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>[8, 8, 8, 16, 28, 56, 148, 288, 476, 968, 1988, 4528, 7756]</t>
+          <t>[6, 6, 15, 22, 21, 87, 97, 214, 510, 1151, 2118, 4123, 7793]</t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>[0, 0, 24, 32, 60, 24, 84, 96, 348, 840, 2244, 4784, 8268]</t>
+          <t>[0, 0, 18, 4, 20, 42, 42, 92, 540, 1090, 2068, 3814, 8008]</t>
         </is>
       </c>
       <c r="J181" t="inlineStr">
@@ -7688,33 +7688,33 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
+        <v>3</v>
+      </c>
+      <c r="C182" t="n">
         <v>4</v>
       </c>
-      <c r="C182" t="n">
-        <v>2</v>
-      </c>
       <c r="D182" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>2.2.ab_c</t>
+          <t>4.2.d_f_k_s</t>
         </is>
       </c>
       <c r="F182" t="n">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="G182" t="n">
-        <v>40</v>
+        <v>351</v>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>[2, 8, 8, 24, 52, 56, 100, 256, 476, 968, 2180, 4272, 8140]</t>
+          <t>[6, 6, 21, 18, 6, 63, 132, 306, 525, 966, 1986, 4191, 8040]</t>
         </is>
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 16, 60, 24, 84, 160, 444, 840, 2244, 4144, 8268]</t>
+          <t>[0, 0, 18, 0, 0, 72, 126, 360, 549, 990, 1683, 4212, 8073]</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
@@ -7728,38 +7728,38 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
+        <v>3</v>
+      </c>
+      <c r="C183" t="n">
         <v>4</v>
       </c>
-      <c r="C183" t="n">
-        <v>2</v>
-      </c>
       <c r="D183" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>2.2.a_c</t>
+          <t>4.2.e_j_q_z</t>
         </is>
       </c>
       <c r="F183" t="n">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="G183" t="n">
-        <v>49</v>
+        <v>513</v>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
+          <t>[7, 7, 13, 19, 17, 85, 77, 291, 589, 1027, 1921, 3949, 8405]</t>
         </is>
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>[0, 6, 3, 34, 30, 15, 126, 226, 471, 1146, 2046, 4063, 8502]</t>
+          <t>[0, 0, 21, 12, 30, 75, 84, 180, 525, 960, 2178, 3963, 8424]</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7768,33 +7768,33 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
+        <v>3</v>
+      </c>
+      <c r="C184" t="n">
         <v>4</v>
       </c>
-      <c r="C184" t="n">
-        <v>2</v>
-      </c>
       <c r="D184" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>2.2.b_a</t>
+          <t>4.2.e_k_u_bg</t>
         </is>
       </c>
       <c r="F184" t="n">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="G184" t="n">
-        <v>16</v>
+        <v>585</v>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>[4, 4, 16, 24, 24, 64, 88, 288, 520, 1104, 2072, 3936, 8168]</t>
+          <t>[7, 9, 13, 9, 17, 81, 161, 225, 481, 1089, 1921, 4353, 7937]</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>[0, 4, 12, 24, 40, 64, 56, 288, 552, 1104, 2200, 4320, 8424]</t>
+          <t>[0, 2, 21, 2, 30, 71, 168, 114, 417, 1022, 2178, 4367, 7956]</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
@@ -7808,33 +7808,33 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
+        <v>3</v>
+      </c>
+      <c r="C185" t="n">
         <v>4</v>
       </c>
-      <c r="C185" t="n">
-        <v>2</v>
-      </c>
       <c r="D185" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>2.2.b_a</t>
+          <t>4.2.f_o_bc_bs</t>
         </is>
       </c>
       <c r="F185" t="n">
-        <v>8</v>
+        <v>260</v>
       </c>
       <c r="G185" t="n">
-        <v>16</v>
+        <v>520</v>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>[4, 4, 16, 24, 24, 64, 88, 288, 520, 1104, 2072, 3936, 8168]</t>
+          <t>[8, 8, 8, 16, 28, 56, 148, 288, 476, 968, 1988, 4528, 7756]</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>[1, 1, 10, 33, 21, 46, 85, 225, 478, 1161, 2069, 4158, 8477]</t>
+          <t>[0, 0, 24, 32, 60, 24, 84, 96, 348, 840, 2244, 4784, 8268]</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
@@ -7858,28 +7858,28 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>2.2.ab_c</t>
         </is>
       </c>
       <c r="F186" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G186" t="n">
         <v>40</v>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[2, 8, 8, 24, 52, 56, 100, 256, 476, 968, 2180, 4272, 8140]</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 24, 30, 56, 126, 256, 582, 968, 2046, 4656, 8502]</t>
+          <t>[0, 0, 12, 16, 60, 24, 84, 160, 444, 840, 2244, 4144, 8268]</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7898,23 +7898,23 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>2.2.b_d</t>
+          <t>2.2.a_c</t>
         </is>
       </c>
       <c r="F187" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G187" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
+          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>[1, 7, 1, 27, 21, 37, 169, 195, 397, 1107, 2069, 4365, 8633]</t>
+          <t>[0, 6, 3, 34, 30, 15, 126, 226, 471, 1146, 2046, 4063, 8502]</t>
         </is>
       </c>
       <c r="J187" t="inlineStr">
@@ -7938,23 +7938,23 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>2.2.b_a</t>
         </is>
       </c>
       <c r="F188" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G188" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[4, 4, 16, 24, 24, 64, 88, 288, 520, 1104, 2072, 3936, 8168]</t>
         </is>
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>[1, 9, 1, 17, 41, 81, 113, 193, 577, 1089, 2113, 4481, 8321]</t>
+          <t>[0, 4, 12, 24, 40, 64, 56, 288, 552, 1104, 2200, 4320, 8424]</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
@@ -7978,23 +7978,23 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>2.2.d_f</t>
+          <t>2.2.b_a</t>
         </is>
       </c>
       <c r="F189" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G189" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+          <t>[4, 4, 16, 24, 24, 64, 88, 288, 520, 1104, 2072, 3936, 8168]</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>[3, 3, 3, 19, 33, 69, 87, 211, 471, 1143, 1917, 4333, 8739]</t>
+          <t>[1, 1, 10, 33, 21, 46, 85, 225, 478, 1161, 2069, 4158, 8477]</t>
         </is>
       </c>
       <c r="J189" t="inlineStr">
@@ -8011,30 +8011,30 @@
         <v>4</v>
       </c>
       <c r="C190" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D190" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>3.2.c_e_f</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F190" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="G190" t="n">
-        <v>216</v>
+        <v>40</v>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>[5, 9, 8, 25, 25, 54, 103, 305, 584, 909, 2117, 3982, 7987]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 28, 0, 36, 84, 308, 540, 900, 1848, 3688, 8112]</t>
+          <t>[0, 8, 6, 24, 30, 56, 126, 256, 582, 968, 2046, 4656, 8502]</t>
         </is>
       </c>
       <c r="J190" t="inlineStr">
@@ -8051,30 +8051,30 @@
         <v>4</v>
       </c>
       <c r="C191" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D191" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>3.2.d_g_i</t>
+          <t>2.2.b_d</t>
         </is>
       </c>
       <c r="F191" t="n">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G191" t="n">
-        <v>200</v>
+        <v>55</v>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>[6, 8, 6, 32, 6, 56, 174, 224, 582, 968, 1854, 4400, 8118]</t>
+          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
         </is>
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>[0, 0, 6, 24, 30, 24, 126, 128, 582, 840, 2046, 4656, 8502]</t>
+          <t>[1, 7, 1, 27, 21, 37, 169, 195, 397, 1107, 2069, 4365, 8633]</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -8091,30 +8091,30 @@
         <v>4</v>
       </c>
       <c r="C192" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D192" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>3.2.d_g_i</t>
+          <t>2.2.c_e</t>
         </is>
       </c>
       <c r="F192" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G192" t="n">
-        <v>200</v>
+        <v>45</v>
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>[6, 8, 6, 32, 6, 56, 174, 224, 582, 968, 1854, 4400, 8118]</t>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>[0, 2, 0, 26, 0, 56, 126, 290, 612, 902, 1716, 4268, 8190]</t>
+          <t>[1, 9, 1, 17, 41, 81, 113, 193, 577, 1089, 2113, 4481, 8321]</t>
         </is>
       </c>
       <c r="J192" t="inlineStr">
@@ -8131,30 +8131,30 @@
         <v>4</v>
       </c>
       <c r="C193" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D193" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>3.2.d_g_k</t>
+          <t>2.2.d_f</t>
         </is>
       </c>
       <c r="F193" t="n">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="G193" t="n">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>[6, 8, 12, 8, 36, 56, 132, 320, 444, 968, 2052, 4400, 7884]</t>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
         </is>
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 28, 35, 60, 168, 252, 459, 1015, 2002, 4756, 8099]</t>
+          <t>[3, 3, 3, 19, 33, 69, 87, 211, 471, 1143, 1917, 4333, 8739]</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
@@ -8171,30 +8171,30 @@
         <v>4</v>
       </c>
       <c r="C194" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D194" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>3.2.d_g_k</t>
+          <t>2.2.c_e</t>
         </is>
       </c>
       <c r="F194" t="n">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="G194" t="n">
-        <v>104</v>
+        <v>45</v>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>[6, 8, 12, 8, 36, 56, 132, 320, 444, 968, 2052, 4400, 7884]</t>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>[0, 2, 0, 26, 30, 20, 126, 194, 360, 1082, 2046, 4844, 8502]</t>
+          <t>[1, 1, 13, 17, 41, 49, 113, 65, 481, 961, 2113, 4097, 8321]</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
@@ -8208,7 +8208,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C195" t="n">
         <v>2</v>
@@ -8218,28 +8218,28 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>2.2.a_a</t>
+          <t>2.2.c_e</t>
         </is>
       </c>
       <c r="F195" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G195" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>[3, 5, 9, 33, 33, 65, 129, 193, 513, 1025, 2049, 4353, 8193]</t>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 20, 15, 90, 105, 180, 540, 1075, 2145, 4130, 8385]</t>
+          <t>[1, 5, 1, 17, 1, 89, 169, 209, 577, 945, 1937, 4097, 7905]</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8248,7 +8248,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C196" t="n">
         <v>2</v>
@@ -8258,23 +8258,23 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>2.2.a_b</t>
+          <t>2.2.d_f</t>
         </is>
       </c>
       <c r="F196" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G196" t="n">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>[3, 7, 9, 31, 33, 43, 129, 223, 513, 1147, 2049, 4111, 8193]</t>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
         </is>
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>[0, 0, 9, 8, 30, 33, 168, 176, 513, 1080, 2178, 3869, 7956]</t>
+          <t>[1, 3, 7, 27, 41, 69, 71, 179, 439, 1143, 1981, 4461, 8867]</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
@@ -8288,38 +8288,38 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C197" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D197" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>3.2.c_e_f</t>
         </is>
       </c>
       <c r="F197" t="n">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G197" t="n">
-        <v>40</v>
+        <v>216</v>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[5, 9, 8, 25, 25, 54, 103, 305, 584, 909, 2117, 3982, 7987]</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>[0, 0, 15, 20, 20, 45, 175, 300, 645, 1090, 1925, 4265, 7995]</t>
+          <t>[0, 0, 0, 28, 0, 36, 84, 308, 540, 900, 1848, 3688, 8112]</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8328,33 +8328,33 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C198" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D198" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>3.2.d_g_i</t>
         </is>
       </c>
       <c r="F198" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G198" t="n">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[6, 8, 6, 32, 6, 56, 174, 224, 582, 968, 1854, 4400, 8118]</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>[0, 6, 0, 18, 0, 60, 210, 242, 540, 1086, 1980, 4380, 8190]</t>
+          <t>[0, 0, 6, 24, 30, 24, 126, 128, 582, 840, 2046, 4656, 8502]</t>
         </is>
       </c>
       <c r="J198" t="inlineStr">
@@ -8368,33 +8368,33 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C199" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D199" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>2.2.b_d</t>
+          <t>3.2.d_g_i</t>
         </is>
       </c>
       <c r="F199" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G199" t="n">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
+          <t>[6, 8, 6, 32, 6, 56, 174, 224, 582, 968, 1854, 4400, 8118]</t>
         </is>
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>[0, 2, 15, 18, 40, 23, 140, 130, 375, 922, 2200, 4143, 8580]</t>
+          <t>[0, 2, 0, 26, 0, 56, 126, 290, 612, 902, 1716, 4268, 8190]</t>
         </is>
       </c>
       <c r="J199" t="inlineStr">
@@ -8408,33 +8408,33 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C200" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D200" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>3.2.d_g_k</t>
         </is>
       </c>
       <c r="F200" t="n">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="G200" t="n">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[6, 8, 12, 8, 36, 56, 132, 320, 444, 968, 2052, 4400, 7884]</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>[0, 6, 3, 34, 30, 63, 126, 98, 471, 1146, 2046, 4447, 8502]</t>
+          <t>[0, 0, 0, 28, 35, 60, 168, 252, 459, 1015, 2002, 4756, 8099]</t>
         </is>
       </c>
       <c r="J200" t="inlineStr">
@@ -8448,38 +8448,38 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C201" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D201" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>3.2.d_g_k</t>
         </is>
       </c>
       <c r="F201" t="n">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="G201" t="n">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[6, 8, 12, 8, 36, 56, 132, 320, 444, 968, 2052, 4400, 7884]</t>
         </is>
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 10, 25, 70, 140, 210, 450, 845, 1870, 4090, 7800]</t>
+          <t>[0, 2, 0, 26, 30, 20, 126, 194, 360, 1082, 2046, 4844, 8502]</t>
         </is>
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8498,28 +8498,28 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>2.2.d_f</t>
+          <t>2.2.a_a</t>
         </is>
       </c>
       <c r="F202" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G202" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+          <t>[3, 5, 9, 33, 33, 65, 129, 193, 513, 1025, 2049, 4353, 8193]</t>
         </is>
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>[1, 3, 7, 27, 41, 69, 71, 179, 439, 1143, 1981, 4461, 8867]</t>
+          <t>[0, 0, 0, 20, 15, 90, 105, 180, 540, 1075, 2145, 4130, 8385]</t>
         </is>
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8528,33 +8528,33 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
+        <v>5</v>
+      </c>
+      <c r="C203" t="n">
+        <v>2</v>
+      </c>
+      <c r="D203" t="n">
         <v>6</v>
       </c>
-      <c r="C203" t="n">
-        <v>2</v>
-      </c>
-      <c r="D203" t="n">
-        <v>7</v>
-      </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>2.2.a_b</t>
         </is>
       </c>
       <c r="F203" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G203" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[3, 7, 9, 31, 33, 43, 129, 223, 513, 1147, 2049, 4111, 8193]</t>
         </is>
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
+          <t>[0, 0, 9, 8, 30, 33, 168, 176, 513, 1080, 2178, 3869, 7956]</t>
         </is>
       </c>
       <c r="J203" t="inlineStr">
@@ -8568,38 +8568,38 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
+        <v>5</v>
+      </c>
+      <c r="C204" t="n">
+        <v>2</v>
+      </c>
+      <c r="D204" t="n">
         <v>6</v>
       </c>
-      <c r="C204" t="n">
-        <v>2</v>
-      </c>
-      <c r="D204" t="n">
-        <v>7</v>
-      </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>2.2.c_c</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F204" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G204" t="n">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>[0, 0, 3, 12, 35, 87, 168, 316, 570, 1015, 2002, 4743, 8099]</t>
+          <t>[0, 0, 15, 20, 20, 45, 175, 300, 645, 1090, 1925, 4265, 7995]</t>
         </is>
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8608,33 +8608,33 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
+        <v>5</v>
+      </c>
+      <c r="C205" t="n">
+        <v>2</v>
+      </c>
+      <c r="D205" t="n">
         <v>6</v>
       </c>
-      <c r="C205" t="n">
-        <v>2</v>
-      </c>
-      <c r="D205" t="n">
-        <v>7</v>
-      </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>2.2.c_c</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F205" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G205" t="n">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 4, 15, 90, 105, 244, 444, 1075, 2145, 4258, 8385]</t>
+          <t>[0, 6, 0, 18, 0, 60, 210, 242, 540, 1086, 1980, 4380, 8190]</t>
         </is>
       </c>
       <c r="J205" t="inlineStr">
@@ -8648,33 +8648,33 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
+        <v>5</v>
+      </c>
+      <c r="C206" t="n">
+        <v>2</v>
+      </c>
+      <c r="D206" t="n">
         <v>6</v>
       </c>
-      <c r="C206" t="n">
-        <v>2</v>
-      </c>
-      <c r="D206" t="n">
-        <v>7</v>
-      </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>2.2.c_c</t>
+          <t>2.2.b_d</t>
         </is>
       </c>
       <c r="F206" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G206" t="n">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
+          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
         </is>
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>[0, 2, 3, 10, 30, 47, 126, 258, 471, 1082, 2046, 4831, 8502]</t>
+          <t>[0, 2, 15, 18, 40, 23, 140, 130, 375, 922, 2200, 4143, 8580]</t>
         </is>
       </c>
       <c r="J206" t="inlineStr">
@@ -8688,33 +8688,33 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
+        <v>5</v>
+      </c>
+      <c r="C207" t="n">
+        <v>2</v>
+      </c>
+      <c r="D207" t="n">
         <v>6</v>
       </c>
-      <c r="C207" t="n">
-        <v>2</v>
-      </c>
-      <c r="D207" t="n">
-        <v>7</v>
-      </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>2.2.c_d</t>
+          <t>2.2.c_e</t>
         </is>
       </c>
       <c r="F207" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G207" t="n">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>[5, 7, 11, 15, 15, 91, 131, 255, 479, 987, 2227, 3999, 8143]</t>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
         </is>
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>[0, 2, 6, 10, 5, 116, 91, 210, 474, 1037, 2387, 3904, 8463]</t>
+          <t>[0, 6, 3, 34, 30, 63, 126, 98, 471, 1146, 2046, 4447, 8502]</t>
         </is>
       </c>
       <c r="J207" t="inlineStr">
@@ -8728,13 +8728,13 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
+        <v>5</v>
+      </c>
+      <c r="C208" t="n">
+        <v>2</v>
+      </c>
+      <c r="D208" t="n">
         <v>6</v>
-      </c>
-      <c r="C208" t="n">
-        <v>2</v>
-      </c>
-      <c r="D208" t="n">
-        <v>7</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -8754,12 +8754,12 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>[0, 2, 9, 2, 30, 71, 168, 114, 513, 1022, 2178, 3983, 7956]</t>
+          <t>[0, 10, 0, 10, 25, 70, 140, 210, 450, 845, 1870, 4090, 7800]</t>
         </is>
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8768,33 +8768,33 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
+        <v>5</v>
+      </c>
+      <c r="C209" t="n">
+        <v>2</v>
+      </c>
+      <c r="D209" t="n">
         <v>6</v>
       </c>
-      <c r="C209" t="n">
-        <v>2</v>
-      </c>
-      <c r="D209" t="n">
-        <v>7</v>
-      </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>2.2.d_f</t>
         </is>
       </c>
       <c r="F209" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G209" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>[0, 4, 0, 12, 15, 106, 105, 148, 540, 1139, 2145, 4002, 8385]</t>
+          <t>[1, 3, 7, 27, 41, 69, 71, 179, 439, 1143, 1981, 4461, 8867]</t>
         </is>
       </c>
       <c r="J209" t="inlineStr">
@@ -8818,23 +8818,23 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F210" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G210" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>[1, 1, 1, 1, 41, 49, 113, 129, 577, 961, 2113, 4225, 8321]</t>
+          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
         </is>
       </c>
       <c r="J210" t="inlineStr">
@@ -8858,23 +8858,23 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>2.2.d_f</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F211" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G211" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>[0, 0, 15, 20, 30, 87, 42, 276, 447, 1020, 1782, 3851, 8502]</t>
+          <t>[0, 0, 3, 12, 35, 87, 168, 316, 570, 1015, 2002, 4743, 8099]</t>
         </is>
       </c>
       <c r="J211" t="inlineStr">
@@ -8898,23 +8898,23 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>2.2.d_f</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F212" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G212" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>[0, 2, 3, 14, 35, 131, 168, 286, 570, 1137, 2002, 4259, 8099]</t>
+          <t>[0, 0, 12, 4, 15, 90, 105, 244, 444, 1075, 2145, 4258, 8385]</t>
         </is>
       </c>
       <c r="J212" t="inlineStr">
@@ -8938,23 +8938,23 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>2.2.d_f</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F213" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G213" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>[0, 4, 3, 12, 30, 91, 126, 228, 471, 1204, 2046, 4347, 8502]</t>
+          <t>[0, 2, 3, 10, 30, 47, 126, 258, 471, 1082, 2046, 4831, 8502]</t>
         </is>
       </c>
       <c r="J213" t="inlineStr">
@@ -8968,13 +8968,13 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
+        <v>6</v>
+      </c>
+      <c r="C214" t="n">
+        <v>2</v>
+      </c>
+      <c r="D214" t="n">
         <v>7</v>
-      </c>
-      <c r="C214" t="n">
-        <v>2</v>
-      </c>
-      <c r="D214" t="n">
-        <v>8</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -8994,10 +8994,290 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
+          <t>[0, 2, 6, 10, 5, 116, 91, 210, 474, 1037, 2387, 3904, 8463]</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>6</v>
+      </c>
+      <c r="C215" t="n">
+        <v>2</v>
+      </c>
+      <c r="D215" t="n">
+        <v>7</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>2.2.c_e</t>
+        </is>
+      </c>
+      <c r="F215" t="n">
+        <v>15</v>
+      </c>
+      <c r="G215" t="n">
+        <v>45</v>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>[0, 2, 9, 2, 30, 71, 168, 114, 513, 1022, 2178, 3983, 7956]</t>
+        </is>
+      </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>6</v>
+      </c>
+      <c r="C216" t="n">
+        <v>2</v>
+      </c>
+      <c r="D216" t="n">
+        <v>7</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>2.2.c_e</t>
+        </is>
+      </c>
+      <c r="F216" t="n">
+        <v>15</v>
+      </c>
+      <c r="G216" t="n">
+        <v>45</v>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>[0, 4, 0, 12, 15, 106, 105, 148, 540, 1139, 2145, 4002, 8385]</t>
+        </is>
+      </c>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>6</v>
+      </c>
+      <c r="C217" t="n">
+        <v>2</v>
+      </c>
+      <c r="D217" t="n">
+        <v>7</v>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>2.2.c_e</t>
+        </is>
+      </c>
+      <c r="F217" t="n">
+        <v>15</v>
+      </c>
+      <c r="G217" t="n">
+        <v>45</v>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>[1, 1, 1, 1, 41, 49, 113, 129, 577, 961, 2113, 4225, 8321]</t>
+        </is>
+      </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>6</v>
+      </c>
+      <c r="C218" t="n">
+        <v>2</v>
+      </c>
+      <c r="D218" t="n">
+        <v>7</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>2.2.d_f</t>
+        </is>
+      </c>
+      <c r="F218" t="n">
+        <v>19</v>
+      </c>
+      <c r="G218" t="n">
+        <v>19</v>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>[0, 0, 15, 20, 30, 87, 42, 276, 447, 1020, 1782, 3851, 8502]</t>
+        </is>
+      </c>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>6</v>
+      </c>
+      <c r="C219" t="n">
+        <v>2</v>
+      </c>
+      <c r="D219" t="n">
+        <v>7</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>2.2.d_f</t>
+        </is>
+      </c>
+      <c r="F219" t="n">
+        <v>19</v>
+      </c>
+      <c r="G219" t="n">
+        <v>19</v>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>[0, 2, 3, 14, 35, 131, 168, 286, 570, 1137, 2002, 4259, 8099]</t>
+        </is>
+      </c>
+      <c r="J219" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>6</v>
+      </c>
+      <c r="C220" t="n">
+        <v>2</v>
+      </c>
+      <c r="D220" t="n">
+        <v>7</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>2.2.d_f</t>
+        </is>
+      </c>
+      <c r="F220" t="n">
+        <v>19</v>
+      </c>
+      <c r="G220" t="n">
+        <v>19</v>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>[0, 4, 3, 12, 30, 91, 126, 228, 471, 1204, 2046, 4347, 8502]</t>
+        </is>
+      </c>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>7</v>
+      </c>
+      <c r="C221" t="n">
+        <v>2</v>
+      </c>
+      <c r="D221" t="n">
+        <v>8</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>2.2.c_d</t>
+        </is>
+      </c>
+      <c r="F221" t="n">
+        <v>14</v>
+      </c>
+      <c r="G221" t="n">
+        <v>28</v>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>[5, 7, 11, 15, 15, 91, 131, 255, 479, 987, 2227, 3999, 8143]</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
           <t>[0, 0, 0, 0, 0, 84, 133, 336, 378, 980, 2310, 4032, 8008]</t>
         </is>
       </c>
-      <c r="J214" t="inlineStr">
+      <c r="J221" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>

<commit_message>
Updated Part I calculations
</commit_message>
<xml_diff>
--- a/Shared/polys.xlsx
+++ b/Shared/polys.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J208"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2654,27 +2654,27 @@
         <v>4</v>
       </c>
       <c r="D56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>4.2.c_g_i_q</t>
+          <t>4.2.c_g_j_q</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G56" t="n">
-        <v>2205</v>
+        <v>1944</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>[5, 13, 5, 25, 25, 49, 145, 225, 545, 1153, 1985, 3841, 8065]</t>
+          <t>[5, 13, 8, 17, 25, 70, 103, 273, 584, 973, 2117, 3854, 7987]</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>[1, 9, 1, 25, 1, 57, 169, 241, 577, 1009, 1937, 3841, 7905]</t>
+          <t>[2, 10, 2, 26, 22, 52, 100, 210, 542, 1030, 2114, 4076, 8296]</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -2698,23 +2698,23 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>4.2.d_h_l_r</t>
+          <t>4.2.c_g_i_q</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="G57" t="n">
-        <v>1161</v>
+        <v>2205</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>[6, 10, 6, 26, 31, 58, 90, 274, 564, 1085, 2030, 3842, 8482]</t>
+          <t>[5, 13, 5, 25, 25, 49, 145, 225, 545, 1153, 1985, 3841, 8065]</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>[1, 11, 1, 19, 31, 47, 85, 291, 469, 841, 1915, 3835, 8217]</t>
+          <t>[1, 9, 1, 25, 1, 57, 169, 241, 577, 1009, 1937, 3841, 7905]</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -2738,28 +2738,28 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>4.2.d_i_o_x</t>
+          <t>4.2.d_h_l_r</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="G58" t="n">
-        <v>1639</v>
+        <v>1161</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>[6, 12, 6, 20, 21, 66, 125, 276, 546, 1007, 1997, 3818, 8703]</t>
+          <t>[6, 10, 6, 26, 31, 58, 90, 274, 564, 1085, 2030, 3842, 8482]</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>[1, 11, 1, 23, 21, 47, 155, 343, 541, 1001, 1937, 3611, 8893]</t>
+          <t>[1, 11, 1, 19, 31, 47, 85, 291, 469, 841, 1915, 3835, 8217]</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -2771,30 +2771,30 @@
         <v>2</v>
       </c>
       <c r="C59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D59" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5.2.ab_d_b_b_j</t>
+          <t>4.2.d_i_o_x</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>60</v>
+        <v>149</v>
       </c>
       <c r="G59" t="n">
-        <v>3960</v>
+        <v>1639</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>[2, 10, 20, 18, 42, 76, 86, 258, 452, 1050, 2026, 4380, 8062]</t>
+          <t>[6, 12, 6, 20, 21, 66, 125, 276, 546, 1007, 1997, 3818, 8703]</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>[0, 4, 0, 20, 20, 40, 112, 196, 432, 1164, 1892, 4568, 8424]</t>
+          <t>[1, 11, 1, 23, 21, 47, 155, 343, 541, 1001, 1937, 3611, 8893]</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -2818,28 +2818,28 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5.2.a_c_d_e_g</t>
+          <t>5.2.ab_d_b_b_j</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="G60" t="n">
-        <v>3528</v>
+        <v>3960</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>[3, 9, 18, 25, 33, 54, 129, 289, 378, 1089, 2049, 4078, 8193]</t>
+          <t>[2, 10, 20, 18, 42, 76, 86, 258, 452, 1050, 2026, 4380, 8062]</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>[0, 6, 0, 18, 30, 36, 126, 290, 432, 1146, 2046, 4428, 8502]</t>
+          <t>[0, 4, 0, 20, 20, 40, 112, 196, 432, 1164, 1892, 4568, 8424]</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2858,23 +2858,23 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>5.2.a_d_c_j_d</t>
+          <t>5.2.a_c_d_e_g</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="G61" t="n">
-        <v>7400</v>
+        <v>3528</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>[3, 11, 15, 35, 18, 53, 122, 227, 483, 1086, 2280, 3977, 8128]</t>
+          <t>[3, 9, 18, 25, 33, 54, 129, 289, 378, 1089, 2049, 4078, 8193]</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>[0, 6, 6, 22, 0, 78, 98, 214, 510, 1136, 2376, 3754, 8320]</t>
+          <t>[0, 6, 0, 18, 30, 36, 126, 290, 432, 1146, 2046, 4428, 8502]</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
@@ -2898,28 +2898,28 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>5.2.b_c_e_i_i</t>
+          <t>5.2.a_d_c_j_d</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G62" t="n">
-        <v>3600</v>
+        <v>7400</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>[4, 8, 16, 32, 24, 80, 88, 192, 520, 1168, 2072, 4064, 8168]</t>
+          <t>[3, 11, 15, 35, 18, 53, 122, 227, 483, 1086, 2280, 3977, 8128]</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 16, 40, 80, 56, 256, 648, 1168, 2200, 4576, 8424]</t>
+          <t>[0, 6, 6, 22, 0, 78, 98, 214, 510, 1136, 2376, 3754, 8320]</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -2938,28 +2938,28 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>5.2.b_d_d_h_d</t>
+          <t>5.2.b_c_e_i_i</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G63" t="n">
-        <v>5336</v>
+        <v>3600</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>[4, 10, 10, 26, 14, 100, 172, 210, 478, 930, 2006, 4076, 8272]</t>
+          <t>[4, 8, 16, 32, 24, 80, 88, 192, 520, 1168, 2072, 4064, 8168]</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 20, 0, 104, 224, 196, 468, 1048, 2068, 4184, 8216]</t>
+          <t>[0, 8, 0, 16, 40, 80, 56, 256, 648, 1168, 2200, 4576, 8424]</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2978,23 +2978,23 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5.2.b_d_d_h_f</t>
+          <t>5.2.b_d_d_h_d</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G64" t="n">
-        <v>5192</v>
+        <v>5336</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>[4, 10, 10, 26, 24, 88, 144, 242, 478, 990, 1896, 3884, 8844]</t>
+          <t>[4, 10, 10, 26, 14, 100, 172, 210, 478, 930, 2006, 4076, 8272]</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 20, 10, 92, 196, 228, 468, 1108, 1958, 3992, 8788]</t>
+          <t>[0, 8, 0, 20, 0, 104, 224, 196, 468, 1048, 2068, 4184, 8216]</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -3018,23 +3018,23 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>5.2.b_d_d_h_h</t>
+          <t>5.2.b_d_d_h_f</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G65" t="n">
-        <v>5040</v>
+        <v>5192</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>[4, 10, 10, 26, 34, 76, 116, 274, 478, 1010, 1874, 3836, 9000]</t>
+          <t>[4, 10, 10, 26, 24, 88, 144, 242, 478, 990, 1896, 3884, 8844]</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 20, 20, 80, 168, 260, 468, 1128, 1936, 3944, 8944]</t>
+          <t>[0, 8, 0, 20, 10, 92, 196, 228, 468, 1108, 1958, 3992, 8788]</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
@@ -3058,23 +3058,23 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>5.2.b_d_d_h_j</t>
+          <t>5.2.b_d_d_h_h</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G66" t="n">
-        <v>4880</v>
+        <v>5040</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>[4, 10, 10, 26, 44, 64, 88, 306, 478, 990, 1940, 3932, 8740]</t>
+          <t>[4, 10, 10, 26, 34, 76, 116, 274, 478, 1010, 1874, 3836, 9000]</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 20, 30, 68, 140, 292, 468, 1108, 2002, 4040, 8684]</t>
+          <t>[0, 8, 0, 20, 20, 80, 168, 260, 468, 1128, 1936, 3944, 8944]</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
@@ -3098,23 +3098,23 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>5.2.b_d_d_j_h</t>
+          <t>5.2.b_d_d_h_j</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G67" t="n">
-        <v>6048</v>
+        <v>4880</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>[4, 10, 10, 34, 24, 76, 116, 194, 586, 1010, 1896, 4060, 8532]</t>
+          <t>[4, 10, 10, 26, 44, 64, 88, 306, 478, 990, 1940, 3932, 8740]</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 28, 10, 80, 168, 180, 576, 1128, 1958, 4168, 8476]</t>
+          <t>[0, 8, 0, 20, 30, 68, 140, 292, 468, 1108, 2002, 4040, 8684]</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -3138,23 +3138,23 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>5.2.b_d_d_j_j</t>
+          <t>5.2.b_d_d_j_h</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G68" t="n">
-        <v>5888</v>
+        <v>6048</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>[4, 10, 10, 34, 34, 64, 88, 226, 550, 1070, 2006, 3964, 8688]</t>
+          <t>[4, 10, 10, 34, 24, 76, 116, 194, 586, 1010, 1896, 4060, 8532]</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 28, 20, 68, 140, 212, 540, 1188, 2068, 4072, 8632]</t>
+          <t>[0, 8, 0, 28, 10, 80, 168, 180, 576, 1128, 1958, 4168, 8476]</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
@@ -3178,23 +3178,23 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>5.2.b_d_d_j_l</t>
+          <t>5.2.b_d_d_j_j</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G69" t="n">
-        <v>5720</v>
+        <v>5888</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>[4, 10, 10, 34, 44, 52, 60, 258, 514, 1090, 2204, 4012, 8428]</t>
+          <t>[4, 10, 10, 34, 34, 64, 88, 226, 550, 1070, 2006, 3964, 8688]</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 28, 30, 56, 112, 244, 504, 1208, 2266, 4120, 8372]</t>
+          <t>[0, 8, 0, 28, 20, 68, 140, 212, 540, 1188, 2068, 4072, 8632]</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
@@ -3218,23 +3218,23 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>5.2.b_d_f_j_j</t>
+          <t>5.2.b_d_d_j_l</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G70" t="n">
-        <v>4968</v>
+        <v>5720</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>[4, 10, 16, 26, 14, 76, 144, 242, 412, 1050, 2050, 4220, 8584]</t>
+          <t>[4, 10, 10, 34, 44, 52, 60, 258, 514, 1090, 2204, 4012, 8428]</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 20, 0, 80, 196, 228, 402, 1168, 2112, 4328, 8528]</t>
+          <t>[0, 8, 0, 28, 30, 56, 112, 244, 504, 1208, 2266, 4120, 8372]</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -3258,23 +3258,23 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>5.2.b_d_f_j_l</t>
+          <t>5.2.b_d_f_j_j</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G71" t="n">
-        <v>4760</v>
+        <v>4968</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>[4, 10, 16, 26, 24, 64, 116, 242, 448, 1190, 1984, 3980, 8532]</t>
+          <t>[4, 10, 16, 26, 14, 76, 144, 242, 412, 1050, 2050, 4220, 8584]</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 20, 10, 68, 168, 228, 438, 1308, 2046, 4088, 8476]</t>
+          <t>[0, 8, 6, 20, 0, 80, 196, 228, 402, 1168, 2112, 4328, 8528]</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
@@ -3298,23 +3298,23 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>5.2.b_e_c_i_a</t>
+          <t>5.2.b_d_f_j_l</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="G72" t="n">
-        <v>7920</v>
+        <v>4760</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>[4, 12, 4, 24, 24, 96, 200, 160, 472, 1072, 1896, 4128, 7960]</t>
+          <t>[4, 10, 16, 26, 24, 64, 116, 242, 448, 1190, 1984, 3980, 8532]</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 24, 0, 104, 224, 176, 504, 928, 1848, 4128, 7800]</t>
+          <t>[0, 8, 6, 20, 10, 68, 168, 228, 438, 1308, 2046, 4088, 8476]</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
@@ -3338,23 +3338,23 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>5.2.b_e_c_i_c</t>
+          <t>5.2.b_e_c_i_a</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G73" t="n">
-        <v>7808</v>
+        <v>7920</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>[4, 12, 4, 24, 34, 84, 158, 240, 490, 912, 1962, 4080, 8402]</t>
+          <t>[4, 12, 4, 24, 24, 96, 200, 160, 472, 1072, 1896, 4128, 7960]</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 24, 10, 92, 182, 256, 522, 768, 1914, 4080, 8242]</t>
+          <t>[0, 8, 0, 24, 0, 104, 224, 176, 504, 928, 1848, 4128, 7800]</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
@@ -3378,23 +3378,23 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>5.2.b_e_c_k_e</t>
+          <t>5.2.b_e_c_i_c</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G74" t="n">
-        <v>8840</v>
+        <v>7808</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>[4, 12, 4, 32, 34, 60, 158, 224, 526, 952, 1742, 4352, 8662]</t>
+          <t>[4, 12, 4, 24, 34, 84, 158, 240, 490, 912, 1962, 4080, 8402]</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 32, 10, 68, 182, 240, 558, 808, 1694, 4352, 8502]</t>
+          <t>[0, 8, 0, 24, 10, 92, 182, 256, 522, 768, 1914, 4080, 8242]</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
@@ -3418,23 +3418,23 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>5.2.b_e_e_k_i</t>
+          <t>5.2.b_e_c_k_e</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="G75" t="n">
-        <v>7776</v>
+        <v>8840</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>[4, 12, 10, 24, 24, 84, 144, 224, 424, 992, 2160, 3984, 8688]</t>
+          <t>[4, 12, 4, 32, 34, 60, 158, 224, 526, 952, 1742, 4352, 8662]</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 24, 0, 92, 168, 240, 456, 848, 2112, 3984, 8528]</t>
+          <t>[0, 8, 0, 32, 10, 68, 182, 240, 558, 808, 1694, 4352, 8502]</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -3458,23 +3458,23 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>5.2.b_e_e_k_k</t>
+          <t>5.2.b_e_e_k_i</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G76" t="n">
-        <v>7592</v>
+        <v>7776</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>[4, 12, 10, 24, 34, 72, 102, 272, 478, 952, 2094, 3984, 8870]</t>
+          <t>[4, 12, 10, 24, 24, 84, 144, 224, 424, 992, 2160, 3984, 8688]</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 24, 10, 80, 126, 288, 510, 808, 2046, 3984, 8710]</t>
+          <t>[0, 8, 6, 24, 0, 92, 168, 240, 456, 848, 2112, 3984, 8528]</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
@@ -3498,23 +3498,23 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>5.2.b_e_e_k_m</t>
+          <t>5.2.b_e_e_k_k</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G77" t="n">
-        <v>7400</v>
+        <v>7592</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>[4, 12, 10, 24, 44, 60, 60, 320, 532, 872, 2116, 4224, 8428]</t>
+          <t>[4, 12, 10, 24, 34, 72, 102, 272, 478, 952, 2094, 3984, 8870]</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 24, 20, 68, 84, 336, 564, 728, 2068, 4224, 8268]</t>
+          <t>[0, 8, 6, 24, 10, 80, 126, 288, 510, 808, 2046, 3984, 8710]</t>
         </is>
       </c>
       <c r="J77" t="inlineStr">
@@ -3538,23 +3538,23 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>5.2.b_e_e_m_k</t>
+          <t>5.2.b_e_e_k_m</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G78" t="n">
-        <v>8816</v>
+        <v>7400</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>[4, 12, 10, 32, 24, 60, 116, 208, 568, 1072, 1984, 4016, 8584]</t>
+          <t>[4, 12, 10, 24, 44, 60, 60, 320, 532, 872, 2116, 4224, 8428]</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 32, 0, 68, 140, 224, 600, 928, 1936, 4016, 8424]</t>
+          <t>[0, 8, 6, 24, 20, 68, 84, 336, 564, 728, 2068, 4224, 8268]</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
@@ -3578,23 +3578,23 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>5.2.b_e_e_m_m</t>
+          <t>5.2.b_e_e_m_k</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G79" t="n">
-        <v>8624</v>
+        <v>8816</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>[4, 12, 10, 32, 34, 48, 74, 256, 586, 1072, 2138, 3872, 8298]</t>
+          <t>[4, 12, 10, 32, 24, 60, 116, 208, 568, 1072, 1984, 4016, 8584]</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 32, 10, 56, 98, 272, 618, 928, 2090, 3872, 8138]</t>
+          <t>[0, 8, 6, 32, 0, 68, 140, 224, 600, 928, 1936, 4016, 8424]</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
@@ -3618,23 +3618,23 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>5.2.b_e_g_m_q</t>
+          <t>5.2.b_e_e_m_m</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="G80" t="n">
-        <v>7056</v>
+        <v>8624</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>[4, 12, 16, 24, 24, 48, 88, 288, 520, 1232, 2072, 3552, 8168]</t>
+          <t>[4, 12, 10, 32, 34, 48, 74, 256, 586, 1072, 2138, 3872, 8298]</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>[0, 8, 12, 24, 0, 56, 112, 304, 552, 1088, 2024, 3552, 8008]</t>
+          <t>[0, 8, 6, 32, 10, 56, 98, 272, 618, 928, 2090, 3872, 8138]</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -3658,28 +3658,28 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>5.2.b_f_f_p_l</t>
+          <t>5.2.b_e_g_m_q</t>
         </is>
       </c>
       <c r="F81" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G81" t="n">
-        <v>12320</v>
+        <v>7056</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>[4, 14, 10, 26, 14, 68, 172, 178, 442, 1094, 2226, 4268, 7960]</t>
+          <t>[4, 12, 16, 24, 24, 48, 88, 288, 520, 1232, 2072, 3552, 8168]</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>[0, 8, 12, 28, 0, 68, 140, 212, 408, 1028, 2024, 3880, 7904]</t>
+          <t>[0, 8, 12, 24, 0, 56, 112, 304, 552, 1088, 2024, 3552, 8008]</t>
         </is>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3698,28 +3698,28 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>5.2.b_f_f_p_n</t>
+          <t>5.2.b_f_f_p_l</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G82" t="n">
-        <v>12104</v>
+        <v>12320</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>[4, 14, 10, 26, 24, 56, 116, 242, 550, 1034, 2116, 3980, 8324]</t>
+          <t>[4, 14, 10, 26, 14, 68, 172, 178, 442, 1094, 2226, 4268, 7960]</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>[0, 8, 12, 28, 10, 56, 84, 276, 516, 968, 1914, 3592, 8268]</t>
+          <t>[0, 8, 12, 28, 0, 68, 140, 212, 408, 1028, 2024, 3880, 7904]</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3738,28 +3738,28 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>5.2.b_f_f_p_p</t>
+          <t>5.2.b_f_f_p_n</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G83" t="n">
-        <v>11880</v>
+        <v>12104</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>[4, 14, 10, 26, 34, 44, 60, 306, 658, 934, 2094, 4028, 7856]</t>
+          <t>[4, 14, 10, 26, 24, 56, 116, 242, 550, 1034, 2116, 3980, 8324]</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>[0, 8, 12, 28, 20, 44, 28, 340, 624, 868, 1892, 3640, 7800]</t>
+          <t>[0, 8, 12, 28, 10, 56, 84, 276, 516, 968, 1914, 3592, 8268]</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3778,28 +3778,28 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>5.2.c_e_e_g_f</t>
+          <t>5.2.b_f_f_p_p</t>
         </is>
       </c>
       <c r="F84" t="n">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="G84" t="n">
-        <v>4088</v>
+        <v>11880</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 25, 30, 93, 145, 273, 491, 884, 1963, 4201, 8273]</t>
+          <t>[4, 14, 10, 26, 34, 44, 60, 306, 658, 934, 2094, 4028, 7856]</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 18, 30, 82, 140, 290, 396, 640, 1848, 4194, 8008]</t>
+          <t>[0, 8, 12, 28, 20, 44, 28, 340, 624, 868, 1892, 3640, 7800]</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3818,23 +3818,23 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>5.2.c_e_e_g_h</t>
+          <t>5.2.c_e_e_g_f</t>
         </is>
       </c>
       <c r="F85" t="n">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G85" t="n">
-        <v>3848</v>
+        <v>4088</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 25, 40, 69, 145, 337, 383, 924, 2051, 4009, 8377]</t>
+          <t>[5, 9, 5, 25, 30, 93, 145, 273, 491, 884, 1963, 4201, 8273]</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 18, 40, 58, 140, 354, 288, 680, 1936, 4002, 8112]</t>
+          <t>[0, 10, 0, 18, 30, 82, 140, 290, 396, 640, 1848, 4194, 8008]</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
@@ -3858,23 +3858,23 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>5.2.c_e_e_i_j</t>
+          <t>5.2.c_e_e_g_h</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G86" t="n">
-        <v>4680</v>
+        <v>3848</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 33, 30, 69, 145, 289, 473, 844, 2007, 4137, 8429]</t>
+          <t>[5, 9, 5, 25, 40, 69, 145, 337, 383, 924, 2051, 4009, 8377]</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 30, 58, 140, 306, 378, 600, 1892, 4130, 8164]</t>
+          <t>[0, 10, 0, 18, 40, 58, 140, 354, 288, 680, 1936, 4002, 8112]</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -3898,23 +3898,23 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>5.2.c_e_e_k_n</t>
+          <t>5.2.c_e_e_i_j</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G87" t="n">
-        <v>5312</v>
+        <v>4680</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 41, 30, 45, 145, 273, 455, 964, 2051, 3881, 8689]</t>
+          <t>[5, 9, 5, 33, 30, 69, 145, 289, 473, 844, 2007, 4137, 8429]</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 34, 30, 34, 140, 290, 360, 720, 1936, 3874, 8424]</t>
+          <t>[0, 10, 0, 26, 30, 58, 140, 306, 378, 600, 1892, 4130, 8164]</t>
         </is>
       </c>
       <c r="J87" t="inlineStr">
@@ -3938,23 +3938,23 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>5.2.c_e_f_k_m</t>
+          <t>5.2.c_e_e_k_n</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G88" t="n">
-        <v>4760</v>
+        <v>5312</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>[5, 9, 8, 33, 25, 78, 117, 257, 548, 809, 1985, 4350, 8429]</t>
+          <t>[5, 9, 5, 41, 30, 45, 145, 273, 455, 964, 2051, 3881, 8689]</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 18, 30, 100, 140, 306, 612, 870, 2178, 4620, 8320]</t>
+          <t>[0, 10, 0, 34, 30, 34, 140, 290, 360, 720, 1936, 3874, 8424]</t>
         </is>
       </c>
       <c r="J88" t="inlineStr">
@@ -3978,28 +3978,28 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>5.2.c_e_f_k_o</t>
+          <t>5.2.c_e_f_k_m</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G89" t="n">
-        <v>4472</v>
+        <v>4760</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>[5, 9, 8, 33, 35, 54, 117, 305, 440, 949, 2007, 4110, 8689]</t>
+          <t>[5, 9, 8, 33, 25, 78, 117, 257, 548, 809, 1985, 4350, 8429]</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 18, 40, 76, 140, 354, 504, 1010, 2200, 4380, 8580]</t>
+          <t>[0, 10, 0, 18, 30, 100, 140, 306, 612, 870, 2178, 4620, 8320]</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4018,28 +4018,28 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>5.2.c_e_f_m_q</t>
+          <t>5.2.c_e_f_k_o</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G90" t="n">
-        <v>5400</v>
+        <v>4472</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>[5, 9, 8, 41, 25, 54, 103, 241, 584, 909, 2117, 4238, 7987]</t>
+          <t>[5, 9, 8, 33, 35, 54, 117, 305, 440, 949, 2007, 4110, 8689]</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 30, 76, 126, 290, 648, 970, 2310, 4508, 7878]</t>
+          <t>[0, 10, 0, 18, 40, 76, 140, 354, 504, 1010, 2200, 4380, 8580]</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4058,23 +4058,23 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>5.2.c_e_g_k_l</t>
+          <t>5.2.c_e_f_m_q</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="G91" t="n">
-        <v>4176</v>
+        <v>5400</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 25, 20, 105, 117, 225, 515, 884, 2007, 4249, 8611]</t>
+          <t>[5, 9, 8, 41, 25, 54, 103, 241, 584, 909, 2117, 4238, 7987]</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 18, 20, 94, 112, 242, 420, 640, 1892, 4242, 8346]</t>
+          <t>[0, 10, 0, 26, 30, 76, 126, 290, 648, 970, 2310, 4508, 7878]</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -4098,23 +4098,23 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>5.2.c_e_g_k_n</t>
+          <t>5.2.c_e_g_k_l</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G92" t="n">
-        <v>3872</v>
+        <v>4176</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 25, 30, 81, 117, 257, 479, 964, 1831, 4441, 8715]</t>
+          <t>[5, 9, 11, 25, 20, 105, 117, 225, 515, 884, 2007, 4249, 8611]</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 18, 30, 70, 112, 274, 384, 720, 1716, 4434, 8450]</t>
+          <t>[0, 10, 6, 18, 20, 94, 112, 242, 420, 640, 1892, 4242, 8346]</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
@@ -4138,23 +4138,23 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>5.2.c_e_g_k_p</t>
+          <t>5.2.c_e_g_k_n</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G93" t="n">
-        <v>3560</v>
+        <v>3872</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 25, 40, 57, 117, 289, 443, 1004, 1831, 4441, 8611]</t>
+          <t>[5, 9, 11, 25, 30, 81, 117, 257, 479, 964, 1831, 4441, 8715]</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 18, 40, 46, 112, 306, 348, 760, 1716, 4434, 8346]</t>
+          <t>[0, 10, 6, 18, 30, 70, 112, 274, 384, 720, 1716, 4434, 8450]</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
@@ -4178,23 +4178,23 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>5.2.c_e_g_k_r</t>
+          <t>5.2.c_e_g_k_p</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G94" t="n">
-        <v>3240</v>
+        <v>3560</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 25, 50, 33, 117, 321, 407, 1004, 2007, 4249, 8299]</t>
+          <t>[5, 9, 11, 25, 40, 57, 117, 289, 443, 1004, 1831, 4441, 8611]</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 18, 50, 22, 112, 338, 312, 760, 1892, 4242, 8034]</t>
+          <t>[0, 10, 6, 18, 40, 46, 112, 306, 348, 760, 1716, 4434, 8346]</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -4218,23 +4218,23 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>5.2.c_e_g_m_p</t>
+          <t>5.2.c_e_g_k_r</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G95" t="n">
-        <v>4784</v>
+        <v>3240</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 33, 20, 81, 89, 241, 605, 844, 2051, 4281, 8455]</t>
+          <t>[5, 9, 11, 25, 50, 33, 117, 321, 407, 1004, 2007, 4249, 8299]</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 26, 20, 70, 84, 258, 510, 600, 1936, 4274, 8190]</t>
+          <t>[0, 10, 6, 18, 50, 22, 112, 338, 312, 760, 1892, 4242, 8034]</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
@@ -4258,23 +4258,23 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>5.2.c_e_g_m_r</t>
+          <t>5.2.c_e_g_m_p</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G96" t="n">
-        <v>4464</v>
+        <v>4784</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 33, 30, 57, 89, 273, 533, 1004, 1963, 4281, 8455]</t>
+          <t>[5, 9, 11, 33, 20, 81, 89, 241, 605, 844, 2051, 4281, 8455]</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 26, 30, 46, 84, 290, 438, 760, 1848, 4274, 8190]</t>
+          <t>[0, 10, 6, 26, 20, 70, 84, 258, 510, 600, 1936, 4274, 8190]</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
@@ -4298,23 +4298,23 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>5.2.c_e_g_m_t</t>
+          <t>5.2.c_e_g_m_r</t>
         </is>
       </c>
       <c r="F97" t="n">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G97" t="n">
-        <v>4136</v>
+        <v>4464</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>[5, 9, 11, 33, 40, 33, 89, 305, 461, 1124, 2051, 4089, 8247]</t>
+          <t>[5, 9, 11, 33, 30, 57, 89, 273, 533, 1004, 1963, 4281, 8455]</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 26, 40, 22, 84, 322, 366, 880, 1936, 4082, 7982]</t>
+          <t>[0, 10, 6, 26, 30, 46, 84, 290, 438, 760, 1848, 4274, 8190]</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
@@ -4338,23 +4338,23 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>5.2.c_e_i_o_t</t>
+          <t>5.2.c_e_g_m_t</t>
         </is>
       </c>
       <c r="F98" t="n">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="G98" t="n">
-        <v>3672</v>
+        <v>4136</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>[5, 9, 17, 25, 20, 69, 89, 241, 575, 1124, 1875, 4201, 8221]</t>
+          <t>[5, 9, 11, 33, 40, 33, 89, 305, 461, 1124, 2051, 4089, 8247]</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>[0, 10, 12, 18, 20, 58, 84, 258, 480, 880, 1760, 4194, 7956]</t>
+          <t>[0, 10, 6, 26, 40, 22, 84, 322, 366, 880, 1936, 4082, 7982]</t>
         </is>
       </c>
       <c r="J98" t="inlineStr">
@@ -4378,23 +4378,23 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>5.2.c_e_i_o_v</t>
+          <t>5.2.c_e_i_o_t</t>
         </is>
       </c>
       <c r="F99" t="n">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G99" t="n">
-        <v>3296</v>
+        <v>3672</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>[5, 9, 17, 25, 30, 45, 89, 241, 611, 1204, 1787, 4201, 7909]</t>
+          <t>[5, 9, 17, 25, 20, 69, 89, 241, 575, 1124, 1875, 4201, 8221]</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>[0, 10, 12, 18, 30, 34, 84, 258, 516, 960, 1672, 4194, 7644]</t>
+          <t>[0, 10, 12, 18, 20, 58, 84, 258, 480, 880, 1760, 4194, 7956]</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -4418,23 +4418,23 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>5.2.c_f_g_l_l</t>
+          <t>5.2.c_e_i_o_v</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="G100" t="n">
-        <v>6696</v>
+        <v>3296</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>[5, 11, 5, 27, 30, 89, 138, 211, 491, 906, 2040, 4329, 8390]</t>
+          <t>[5, 9, 17, 25, 30, 45, 89, 241, 611, 1204, 1787, 4201, 7909]</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 30, 30, 70, 168, 278, 486, 900, 1980, 4122, 8580]</t>
+          <t>[0, 10, 12, 18, 30, 34, 84, 258, 516, 960, 1672, 4194, 7644]</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
@@ -4458,23 +4458,23 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>5.2.c_f_g_n_p</t>
+          <t>5.2.c_f_g_l_l</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="G101" t="n">
-        <v>7448</v>
+        <v>6696</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>[5, 11, 5, 35, 30, 53, 138, 259, 473, 886, 2128, 4313, 8416]</t>
+          <t>[5, 11, 5, 27, 30, 89, 138, 211, 491, 906, 2040, 4329, 8390]</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 38, 30, 34, 168, 326, 468, 880, 2068, 4106, 8606]</t>
+          <t>[0, 10, 0, 30, 30, 70, 168, 278, 486, 900, 1980, 4122, 8580]</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
@@ -4498,28 +4498,28 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>5.2.c_f_i_n_r</t>
+          <t>5.2.c_f_g_n_p</t>
         </is>
       </c>
       <c r="F102" t="n">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G102" t="n">
-        <v>5408</v>
+        <v>7448</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 19, 30, 89, 124, 211, 407, 1146, 2040, 4177, 8624]</t>
+          <t>[5, 11, 5, 35, 30, 53, 138, 259, 473, 886, 2128, 4313, 8416]</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 22, 30, 70, 154, 278, 402, 1140, 1980, 3970, 8814]</t>
+          <t>[0, 10, 0, 38, 30, 34, 168, 326, 468, 880, 2068, 4106, 8606]</t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4538,28 +4538,28 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>5.2.c_f_i_n_t</t>
+          <t>5.2.c_f_i_n_r</t>
         </is>
       </c>
       <c r="F103" t="n">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G103" t="n">
-        <v>5040</v>
+        <v>5408</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 19, 40, 65, 110, 275, 407, 1066, 2018, 4369, 8598]</t>
+          <t>[5, 11, 11, 19, 30, 89, 124, 211, 407, 1146, 2040, 4177, 8624]</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 22, 40, 46, 140, 342, 402, 1060, 1958, 4162, 8788]</t>
+          <t>[0, 10, 6, 22, 30, 70, 154, 278, 402, 1140, 1980, 3970, 8814]</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4578,28 +4578,28 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>5.2.c_f_i_p_t</t>
+          <t>5.2.c_f_i_n_t</t>
         </is>
       </c>
       <c r="F104" t="n">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G104" t="n">
-        <v>6480</v>
+        <v>5040</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 27, 20, 77, 110, 227, 533, 1006, 2018, 4305, 8676]</t>
+          <t>[5, 11, 11, 19, 40, 65, 110, 275, 407, 1066, 2018, 4369, 8598]</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 30, 20, 58, 140, 294, 528, 1000, 1958, 4098, 8866]</t>
+          <t>[0, 10, 6, 22, 40, 46, 140, 342, 402, 1060, 1958, 4162, 8788]</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4618,23 +4618,23 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>5.2.c_f_i_p_v</t>
+          <t>5.2.c_f_i_p_t</t>
         </is>
       </c>
       <c r="F105" t="n">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G105" t="n">
-        <v>6104</v>
+        <v>6480</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 27, 30, 53, 96, 291, 497, 1046, 1996, 4209, 8702]</t>
+          <t>[5, 11, 11, 27, 20, 77, 110, 227, 533, 1006, 2018, 4305, 8676]</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 30, 30, 34, 126, 358, 492, 1040, 1936, 4002, 8892]</t>
+          <t>[0, 10, 6, 30, 20, 58, 140, 294, 528, 1000, 1958, 4098, 8866]</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
@@ -4658,28 +4658,28 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>5.2.c_f_k_r_z</t>
+          <t>5.2.c_f_i_p_v</t>
         </is>
       </c>
       <c r="F106" t="n">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="G106" t="n">
-        <v>4760</v>
+        <v>6104</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>[5, 11, 17, 19, 20, 53, 124, 259, 521, 1206, 1798, 4105, 8286]</t>
+          <t>[5, 11, 11, 27, 30, 53, 96, 291, 497, 1046, 1996, 4209, 8702]</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>[0, 10, 12, 22, 20, 34, 154, 326, 516, 1200, 1738, 3898, 8476]</t>
+          <t>[0, 10, 6, 30, 30, 34, 126, 358, 492, 1040, 1936, 4002, 8892]</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4698,23 +4698,23 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>5.2.c_g_i_s_v</t>
+          <t>5.2.c_f_k_r_z</t>
         </is>
       </c>
       <c r="F107" t="n">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G107" t="n">
-        <v>10856</v>
+        <v>4760</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>[5, 13, 5, 33, 30, 37, 131, 273, 491, 948, 2227, 4257, 8065]</t>
+          <t>[5, 11, 17, 19, 20, 53, 124, 259, 521, 1206, 1798, 4105, 8286]</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>[0, 14, 0, 26, 30, 26, 126, 290, 396, 704, 2112, 4250, 7800]</t>
+          <t>[0, 10, 12, 22, 20, 34, 154, 326, 516, 1200, 1738, 3898, 8476]</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
@@ -4738,28 +4738,28 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>5.2.c_g_j_q_u</t>
+          <t>5.2.c_g_i_s_v</t>
         </is>
       </c>
       <c r="F108" t="n">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="G108" t="n">
-        <v>8424</v>
+        <v>10856</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>[5, 13, 8, 17, 35, 94, 103, 193, 440, 1193, 2227, 3710, 8559]</t>
+          <t>[5, 13, 5, 33, 30, 37, 131, 273, 491, 948, 2227, 4257, 8065]</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 34, 40, 76, 84, 98, 366, 1250, 2288, 4060, 8996]</t>
+          <t>[0, 14, 0, 26, 30, 26, 126, 290, 396, 704, 2112, 4250, 7800]</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4778,28 +4778,28 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>5.2.c_g_j_s_w</t>
+          <t>5.2.c_g_j_q_u</t>
         </is>
       </c>
       <c r="F109" t="n">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="G109" t="n">
-        <v>9680</v>
+        <v>8424</v>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>[5, 13, 8, 25, 25, 70, 117, 225, 512, 1033, 2161, 4174, 8429]</t>
+          <t>[5, 13, 8, 17, 35, 94, 103, 193, 440, 1193, 2227, 3710, 8559]</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 42, 30, 52, 98, 130, 438, 1090, 2222, 4524, 8866]</t>
+          <t>[0, 10, 6, 34, 40, 76, 84, 98, 366, 1250, 2288, 4060, 8996]</t>
         </is>
       </c>
       <c r="J109" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4818,23 +4818,23 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>5.2.c_g_j_u_y</t>
+          <t>5.2.c_g_j_s_w</t>
         </is>
       </c>
       <c r="F110" t="n">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G110" t="n">
-        <v>11000</v>
+        <v>9680</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>[5, 13, 8, 33, 15, 46, 131, 225, 656, 993, 1831, 4446, 7987]</t>
+          <t>[5, 13, 8, 25, 25, 70, 117, 225, 512, 1033, 2161, 4174, 8429]</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>[0, 10, 6, 50, 20, 28, 112, 130, 582, 1050, 1892, 4796, 8424]</t>
+          <t>[0, 10, 6, 42, 30, 52, 98, 130, 438, 1090, 2222, 4524, 8866]</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
@@ -4858,23 +4858,23 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>5.2.c_g_l_u_bc</t>
+          <t>5.2.c_g_j_u_y</t>
         </is>
       </c>
       <c r="F111" t="n">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="G111" t="n">
-        <v>7920</v>
+        <v>11000</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>[5, 13, 14, 17, 15, 70, 131, 257, 446, 1193, 2095, 3854, 8299]</t>
+          <t>[5, 13, 8, 33, 15, 46, 131, 225, 656, 993, 1831, 4446, 7987]</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>[0, 10, 12, 34, 20, 52, 112, 162, 372, 1250, 2156, 4204, 8736]</t>
+          <t>[0, 10, 6, 50, 20, 28, 112, 130, 582, 1050, 1892, 4796, 8424]</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
@@ -4898,28 +4898,28 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>5.2.d_h_n_z_bl</t>
+          <t>5.2.c_g_l_u_bc</t>
         </is>
       </c>
       <c r="F112" t="n">
-        <v>324</v>
+        <v>264</v>
       </c>
       <c r="G112" t="n">
-        <v>5832</v>
+        <v>7920</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>[6, 10, 12, 34, 6, 52, 90, 322, 660, 850, 2118, 3820, 7962]</t>
+          <t>[5, 13, 14, 17, 15, 70, 131, 257, 446, 1193, 2095, 3854, 8299]</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>[0, 12, 12, 20, 0, 96, 168, 356, 660, 972, 2376, 3848, 7488]</t>
+          <t>[0, 10, 12, 34, 20, 52, 112, 162, 372, 1250, 2156, 4204, 8736]</t>
         </is>
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4938,28 +4938,28 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>5.2.d_h_o_z_bk</t>
+          <t>5.2.d_h_n_z_bl</t>
         </is>
       </c>
       <c r="F113" t="n">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G113" t="n">
-        <v>4592</v>
+        <v>5832</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>[6, 10, 15, 22, 11, 79, 83, 294, 582, 955, 2052, 4147, 8261]</t>
+          <t>[6, 10, 12, 34, 6, 52, 90, 322, 660, 850, 2118, 3820, 7962]</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
         <is>
-          <t>[0, 12, 18, 20, 10, 66, 28, 236, 612, 1022, 2002, 4094, 8476]</t>
+          <t>[0, 12, 12, 20, 0, 96, 168, 356, 660, 972, 2376, 3848, 7488]</t>
         </is>
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -4978,23 +4978,23 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>5.2.d_h_o_z_bm</t>
+          <t>5.2.d_h_o_z_bk</t>
         </is>
       </c>
       <c r="F114" t="n">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G114" t="n">
-        <v>3960</v>
+        <v>4592</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>[6, 10, 15, 22, 21, 43, 111, 310, 582, 1015, 1788, 4387, 7923]</t>
+          <t>[6, 10, 15, 22, 11, 79, 83, 294, 582, 955, 2052, 4147, 8261]</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>[0, 12, 18, 20, 20, 30, 56, 252, 612, 1082, 1738, 4334, 8138]</t>
+          <t>[0, 12, 18, 20, 10, 66, 28, 236, 612, 1022, 2002, 4094, 8476]</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
@@ -5018,28 +5018,28 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>5.2.d_i_q_bc_bs</t>
+          <t>5.2.d_h_o_z_bm</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>364</v>
+        <v>330</v>
       </c>
       <c r="G115" t="n">
-        <v>5096</v>
+        <v>3960</v>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>[6, 12, 12, 16, 36, 24, 132, 352, 444, 1032, 2052, 4144, 7884]</t>
+          <t>[6, 10, 15, 22, 21, 43, 111, 310, 582, 1015, 1788, 4387, 7923]</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
         <is>
-          <t>[0, 12, 12, 24, 60, 24, 84, 320, 444, 1032, 2244, 4656, 8268]</t>
+          <t>[0, 12, 18, 20, 20, 30, 56, 252, 612, 1082, 1738, 4334, 8138]</t>
         </is>
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5051,35 +5051,35 @@
         <v>2</v>
       </c>
       <c r="C116" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D116" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>6.2.b_f_h_p_t_bk</t>
+          <t>5.2.d_i_q_bc_bs</t>
         </is>
       </c>
       <c r="F116" t="n">
-        <v>414</v>
+        <v>364</v>
       </c>
       <c r="G116" t="n">
-        <v>44712</v>
+        <v>5096</v>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>[4, 14, 16, 18, 14, 92, 144, 210, 412, 1114, 2050, 4092, 8584]</t>
+          <t>[6, 12, 12, 16, 36, 24, 132, 352, 444, 1032, 2052, 4144, 7884]</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 28, 0, 56, 154, 116, 360, 1228, 1980, 4408, 9074]</t>
+          <t>[0, 12, 12, 24, 60, 24, 84, 320, 444, 1032, 2244, 4656, 8268]</t>
         </is>
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5098,23 +5098,23 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>6.2.b_f_h_p_v_bi</t>
+          <t>6.2.b_f_h_p_t_bk</t>
         </is>
       </c>
       <c r="F117" t="n">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G117" t="n">
-        <v>41800</v>
+        <v>44712</v>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>[4, 14, 16, 18, 24, 68, 130, 274, 412, 1054, 1940, 4332, 8870]</t>
+          <t>[4, 14, 16, 18, 14, 92, 144, 210, 412, 1114, 2050, 4092, 8584]</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 28, 10, 32, 140, 180, 360, 1168, 1870, 4648, 9360]</t>
+          <t>[0, 8, 0, 28, 0, 56, 154, 116, 360, 1228, 1980, 4408, 9074]</t>
         </is>
       </c>
       <c r="J117" t="inlineStr">
@@ -5138,23 +5138,23 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>6.2.b_f_h_r_v_bq</t>
+          <t>6.2.b_f_h_p_v_bi</t>
         </is>
       </c>
       <c r="F118" t="n">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="G118" t="n">
-        <v>51448</v>
+        <v>41800</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>[4, 14, 16, 26, 14, 68, 102, 226, 556, 1134, 2050, 4028, 8298]</t>
+          <t>[4, 14, 16, 18, 24, 68, 130, 274, 412, 1054, 1940, 4332, 8870]</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 36, 0, 32, 112, 132, 504, 1248, 1980, 4344, 8788]</t>
+          <t>[0, 8, 0, 28, 10, 32, 140, 180, 360, 1168, 1870, 4648, 9360]</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
@@ -5178,23 +5178,23 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>6.2.b_g_i_v_ba_bz</t>
+          <t>6.2.b_f_h_r_v_bq</t>
         </is>
       </c>
       <c r="F119" t="n">
-        <v>506</v>
+        <v>436</v>
       </c>
       <c r="G119" t="n">
-        <v>70840</v>
+        <v>51448</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>[4, 16, 16, 20, 9, 64, 130, 268, 493, 1071, 2072, 3980, 8675]</t>
+          <t>[4, 14, 16, 26, 14, 68, 102, 226, 556, 1134, 2050, 4028, 8298]</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>[0, 8, 0, 32, 0, 68, 182, 232, 540, 1118, 1958, 4208, 8762]</t>
+          <t>[0, 8, 0, 36, 0, 32, 112, 132, 504, 1248, 1980, 4344, 8788]</t>
         </is>
       </c>
       <c r="J119" t="inlineStr">
@@ -5218,23 +5218,23 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_v_bh</t>
+          <t>6.2.b_g_i_v_ba_bz</t>
         </is>
       </c>
       <c r="F120" t="n">
-        <v>464</v>
+        <v>506</v>
       </c>
       <c r="G120" t="n">
-        <v>28768</v>
+        <v>70840</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 20, 65, 152, 279, 398, 976, 2051, 4105, 8442]</t>
+          <t>[4, 16, 16, 20, 9, 64, 130, 268, 493, 1071, 2072, 3980, 8675]</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 0, 34, 126, 222, 450, 1100, 1870, 4018, 8710]</t>
+          <t>[0, 8, 0, 32, 0, 68, 182, 232, 540, 1118, 1958, 4208, 8762]</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -5258,23 +5258,23 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_v_bj</t>
+          <t>6.2.c_f_i_q_v_bh</t>
         </is>
       </c>
       <c r="F121" t="n">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G121" t="n">
-        <v>29824</v>
+        <v>28768</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 20, 77, 124, 263, 470, 916, 2161, 4033, 8130]</t>
+          <t>[5, 11, 11, 31, 20, 65, 152, 279, 398, 976, 2051, 4105, 8442]</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 0, 46, 98, 206, 522, 1040, 1980, 3946, 8398]</t>
+          <t>[0, 10, 0, 22, 0, 34, 126, 222, 450, 1100, 1870, 4018, 8710]</t>
         </is>
       </c>
       <c r="J121" t="inlineStr">
@@ -5298,23 +5298,23 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_v_bl</t>
+          <t>6.2.c_f_i_q_v_bj</t>
         </is>
       </c>
       <c r="F122" t="n">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G122" t="n">
-        <v>30888</v>
+        <v>29824</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 20, 89, 96, 247, 542, 856, 2271, 3913, 8026]</t>
+          <t>[5, 11, 11, 31, 20, 77, 124, 263, 470, 916, 2161, 4033, 8130]</t>
         </is>
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 0, 58, 70, 190, 594, 980, 2090, 3826, 8294]</t>
+          <t>[0, 10, 0, 22, 0, 46, 98, 206, 522, 1040, 1980, 3946, 8398]</t>
         </is>
       </c>
       <c r="J122" t="inlineStr">
@@ -5338,23 +5338,23 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_x_bj</t>
+          <t>6.2.c_f_i_q_v_bl</t>
         </is>
       </c>
       <c r="F123" t="n">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G123" t="n">
-        <v>27376</v>
+        <v>30888</v>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 30, 53, 138, 263, 380, 1156, 2029, 3937, 8416]</t>
+          <t>[5, 11, 11, 31, 20, 89, 96, 247, 542, 856, 2271, 3913, 8026]</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 10, 22, 112, 206, 432, 1280, 1848, 3850, 8684]</t>
+          <t>[0, 10, 0, 22, 0, 58, 70, 190, 594, 980, 2090, 3826, 8294]</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
@@ -5378,23 +5378,23 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_x_bl</t>
+          <t>6.2.c_f_i_q_x_bj</t>
         </is>
       </c>
       <c r="F124" t="n">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G124" t="n">
-        <v>28440</v>
+        <v>27376</v>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 30, 65, 110, 247, 452, 1096, 2095, 4009, 8104]</t>
+          <t>[5, 11, 11, 31, 30, 53, 138, 263, 380, 1156, 2029, 3937, 8416]</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 10, 34, 84, 190, 504, 1220, 1914, 3922, 8372]</t>
+          <t>[0, 10, 0, 22, 10, 22, 112, 206, 432, 1280, 1848, 3850, 8684]</t>
         </is>
       </c>
       <c r="J124" t="inlineStr">
@@ -5418,23 +5418,23 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_x_bn</t>
+          <t>6.2.c_f_i_q_x_bl</t>
         </is>
       </c>
       <c r="F125" t="n">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G125" t="n">
-        <v>29512</v>
+        <v>28440</v>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 30, 77, 82, 231, 524, 1036, 2161, 4033, 8000]</t>
+          <t>[5, 11, 11, 31, 30, 65, 110, 247, 452, 1096, 2095, 4009, 8104]</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 10, 46, 56, 174, 576, 1160, 1980, 3946, 8268]</t>
+          <t>[0, 10, 0, 22, 10, 34, 84, 190, 504, 1220, 1914, 3922, 8372]</t>
         </is>
       </c>
       <c r="J125" t="inlineStr">
@@ -5458,23 +5458,23 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_x_bp</t>
+          <t>6.2.c_f_i_q_x_bn</t>
         </is>
       </c>
       <c r="F126" t="n">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G126" t="n">
-        <v>30592</v>
+        <v>29512</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 30, 89, 54, 215, 596, 976, 2227, 4009, 8104]</t>
+          <t>[5, 11, 11, 31, 30, 77, 82, 231, 524, 1036, 2161, 4033, 8000]</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 10, 58, 28, 158, 648, 1100, 2046, 3922, 8372]</t>
+          <t>[0, 10, 0, 22, 10, 46, 56, 174, 576, 1160, 1980, 3946, 8268]</t>
         </is>
       </c>
       <c r="J126" t="inlineStr">
@@ -5498,23 +5498,23 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_z_bn</t>
+          <t>6.2.c_f_i_q_x_bp</t>
         </is>
       </c>
       <c r="F127" t="n">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G127" t="n">
-        <v>26992</v>
+        <v>30592</v>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 40, 53, 96, 231, 434, 1236, 2117, 4033, 8078]</t>
+          <t>[5, 11, 11, 31, 30, 89, 54, 215, 596, 976, 2227, 4009, 8104]</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 20, 22, 70, 174, 486, 1360, 1936, 3946, 8346]</t>
+          <t>[0, 10, 0, 22, 10, 58, 28, 158, 648, 1100, 2046, 3922, 8372]</t>
         </is>
       </c>
       <c r="J127" t="inlineStr">
@@ -5538,23 +5538,23 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_q_z_bp</t>
+          <t>6.2.c_f_i_q_z_bn</t>
         </is>
       </c>
       <c r="F128" t="n">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G128" t="n">
-        <v>28072</v>
+        <v>26992</v>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 31, 40, 65, 68, 215, 506, 1176, 2139, 4201, 7974]</t>
+          <t>[5, 11, 11, 31, 40, 53, 96, 231, 434, 1236, 2117, 4033, 8078]</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 22, 20, 34, 42, 158, 558, 1300, 1958, 4114, 8242]</t>
+          <t>[0, 10, 0, 22, 20, 22, 70, 174, 486, 1360, 1936, 3946, 8346]</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
@@ -5578,23 +5578,23 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_s_z_bp</t>
+          <t>6.2.c_f_i_q_z_bp</t>
         </is>
       </c>
       <c r="F129" t="n">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="G129" t="n">
-        <v>33592</v>
+        <v>28072</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 39, 20, 53, 124, 215, 452, 1176, 2227, 3945, 8208]</t>
+          <t>[5, 11, 11, 31, 40, 65, 68, 215, 506, 1176, 2139, 4201, 7974]</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 30, 0, 22, 98, 158, 504, 1300, 2046, 3858, 8476]</t>
+          <t>[0, 10, 0, 22, 20, 34, 42, 158, 558, 1300, 1958, 4114, 8242]</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
@@ -5618,23 +5618,23 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>6.2.c_f_i_s_z_br</t>
+          <t>6.2.c_f_i_s_z_bp</t>
         </is>
       </c>
       <c r="F130" t="n">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G130" t="n">
-        <v>34720</v>
+        <v>33592</v>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>[5, 11, 11, 39, 20, 65, 96, 199, 524, 1076, 2425, 3969, 7688]</t>
+          <t>[5, 11, 11, 39, 20, 53, 124, 215, 452, 1176, 2227, 3945, 8208]</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 30, 0, 34, 70, 142, 576, 1200, 2244, 3882, 7956]</t>
+          <t>[0, 10, 0, 30, 0, 22, 98, 158, 504, 1300, 2046, 3858, 8476]</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
@@ -5658,23 +5658,23 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>6.2.c_g_l_w_bg_ca</t>
+          <t>6.2.c_f_i_s_z_br</t>
         </is>
       </c>
       <c r="F131" t="n">
-        <v>590</v>
+        <v>496</v>
       </c>
       <c r="G131" t="n">
-        <v>40120</v>
+        <v>34720</v>
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>[5, 13, 14, 25, 15, 70, 117, 273, 482, 933, 2139, 4462, 8169]</t>
+          <t>[5, 11, 11, 39, 20, 65, 96, 199, 524, 1076, 2425, 3969, 7688]</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 20, 52, 98, 242, 504, 990, 2200, 4940, 8606]</t>
+          <t>[0, 10, 0, 30, 0, 34, 70, 142, 576, 1200, 2244, 3882, 7956]</t>
         </is>
       </c>
       <c r="J131" t="inlineStr">
@@ -5698,23 +5698,23 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>6.2.c_g_l_w_bg_cc</t>
+          <t>6.2.c_g_l_w_bg_ca</t>
         </is>
       </c>
       <c r="F132" t="n">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="G132" t="n">
-        <v>41440</v>
+        <v>40120</v>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>[5, 13, 14, 25, 15, 82, 89, 241, 572, 973, 2139, 4174, 8117]</t>
+          <t>[5, 13, 14, 25, 15, 70, 117, 273, 482, 933, 2139, 4462, 8169]</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 20, 64, 70, 210, 594, 1030, 2200, 4652, 8554]</t>
+          <t>[0, 10, 0, 26, 20, 52, 98, 242, 504, 990, 2200, 4940, 8606]</t>
         </is>
       </c>
       <c r="J132" t="inlineStr">
@@ -5738,23 +5738,23 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>6.2.c_g_l_w_bg_ce</t>
+          <t>6.2.c_g_l_w_bg_cc</t>
         </is>
       </c>
       <c r="F133" t="n">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G133" t="n">
-        <v>42768</v>
+        <v>41440</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>[5, 13, 14, 25, 15, 94, 61, 209, 662, 1013, 2139, 3838, 8273]</t>
+          <t>[5, 13, 14, 25, 15, 82, 89, 241, 572, 973, 2139, 4174, 8117]</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 20, 76, 42, 178, 684, 1070, 2200, 4316, 8710]</t>
+          <t>[0, 10, 0, 26, 20, 64, 70, 210, 594, 1030, 2200, 4652, 8554]</t>
         </is>
       </c>
       <c r="J133" t="inlineStr">
@@ -5778,23 +5778,23 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>6.2.c_g_l_w_bi_ca</t>
+          <t>6.2.c_g_l_w_bg_ce</t>
         </is>
       </c>
       <c r="F134" t="n">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="G134" t="n">
-        <v>36952</v>
+        <v>42768</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>[5, 13, 14, 25, 25, 46, 117, 289, 446, 1113, 2073, 4222, 8013]</t>
+          <t>[5, 13, 14, 25, 15, 94, 61, 209, 662, 1013, 2139, 3838, 8273]</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 30, 28, 98, 258, 468, 1170, 2134, 4700, 8450]</t>
+          <t>[0, 10, 0, 26, 20, 76, 42, 178, 684, 1070, 2200, 4316, 8710]</t>
         </is>
       </c>
       <c r="J134" t="inlineStr">
@@ -5818,23 +5818,23 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>6.2.c_g_l_w_bi_cc</t>
+          <t>6.2.c_g_l_w_bi_ca</t>
         </is>
       </c>
       <c r="F135" t="n">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="G135" t="n">
-        <v>38272</v>
+        <v>36952</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>[5, 13, 14, 25, 25, 58, 89, 257, 536, 1153, 2029, 4126, 7857]</t>
+          <t>[5, 13, 14, 25, 25, 46, 117, 289, 446, 1113, 2073, 4222, 8013]</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 30, 40, 70, 226, 558, 1210, 2090, 4604, 8294]</t>
+          <t>[0, 10, 0, 26, 30, 28, 98, 258, 468, 1170, 2134, 4700, 8450]</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
@@ -5858,23 +5858,23 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>6.2.c_g_l_w_bi_ce</t>
+          <t>6.2.c_g_l_w_bi_cc</t>
         </is>
       </c>
       <c r="F136" t="n">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G136" t="n">
-        <v>39600</v>
+        <v>38272</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>[5, 13, 14, 25, 25, 70, 61, 225, 626, 1193, 1985, 3982, 7909]</t>
+          <t>[5, 13, 14, 25, 25, 58, 89, 257, 536, 1153, 2029, 4126, 7857]</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 26, 30, 52, 42, 194, 648, 1250, 2046, 4460, 8346]</t>
+          <t>[0, 10, 0, 26, 30, 40, 70, 226, 558, 1210, 2090, 4604, 8294]</t>
         </is>
       </c>
       <c r="J136" t="inlineStr">
@@ -5898,28 +5898,28 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>6.2.c_h_k_z_bd_cg</t>
+          <t>6.2.c_g_l_w_bi_ce</t>
         </is>
       </c>
       <c r="F137" t="n">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="G137" t="n">
-        <v>75640</v>
+        <v>39600</v>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>[5, 15, 5, 35, 20, 45, 180, 195, 455, 1090, 2040, 4265, 8260]</t>
+          <t>[5, 13, 14, 25, 25, 70, 61, 225, 626, 1193, 1985, 3982, 7909]</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 30, 10, 70, 140, 150, 450, 1140, 2200, 4170, 8580]</t>
+          <t>[0, 10, 0, 26, 30, 52, 42, 194, 648, 1250, 2046, 4460, 8346]</t>
         </is>
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -5938,28 +5938,28 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>6.2.d_h_m_x_bi_ca</t>
+          <t>6.2.c_h_k_z_bd_cg</t>
         </is>
       </c>
       <c r="F138" t="n">
-        <v>660</v>
+        <v>610</v>
       </c>
       <c r="G138" t="n">
-        <v>27720</v>
+        <v>75640</v>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>[6, 10, 9, 38, 11, 79, 139, 182, 540, 1055, 1920, 4091, 8547]</t>
+          <t>[5, 15, 5, 35, 20, 45, 180, 195, 455, 1090, 2040, 4265, 8260]</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 20, 10, 66, 84, 188, 666, 1122, 1870, 4166, 8762]</t>
+          <t>[0, 10, 0, 30, 10, 70, 140, 150, 450, 1140, 2200, 4170, 8580]</t>
         </is>
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -5978,23 +5978,23 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>6.2.d_h_m_x_bk_ce</t>
+          <t>6.2.d_h_m_x_bi_ca</t>
         </is>
       </c>
       <c r="F139" t="n">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="G139" t="n">
-        <v>26800</v>
+        <v>27720</v>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>[6, 10, 9, 38, 21, 67, 111, 198, 540, 1155, 1920, 3995, 8625]</t>
+          <t>[6, 10, 9, 38, 11, 79, 139, 182, 540, 1055, 1920, 4091, 8547]</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 20, 20, 54, 56, 204, 666, 1222, 1870, 4070, 8840]</t>
+          <t>[0, 12, 0, 20, 10, 66, 84, 188, 666, 1122, 1870, 4166, 8762]</t>
         </is>
       </c>
       <c r="J139" t="inlineStr">
@@ -6018,23 +6018,23 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>6.2.d_h_m_x_bm_ci</t>
+          <t>6.2.d_h_m_x_bk_ce</t>
         </is>
       </c>
       <c r="F140" t="n">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="G140" t="n">
-        <v>25840</v>
+        <v>26800</v>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>[6, 10, 9, 38, 31, 55, 83, 214, 540, 1215, 2008, 4043, 8391]</t>
+          <t>[6, 10, 9, 38, 21, 67, 111, 198, 540, 1155, 1920, 3995, 8625]</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 20, 30, 42, 28, 220, 666, 1282, 1958, 4118, 8606]</t>
+          <t>[0, 12, 0, 20, 20, 54, 56, 204, 666, 1222, 1870, 4070, 8840]</t>
         </is>
       </c>
       <c r="J140" t="inlineStr">
@@ -6058,23 +6058,23 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>6.2.d_j_r_bh_bx_cy</t>
+          <t>6.2.d_h_m_x_bm_ci</t>
         </is>
       </c>
       <c r="F141" t="n">
-        <v>858</v>
+        <v>680</v>
       </c>
       <c r="G141" t="n">
-        <v>51480</v>
+        <v>25840</v>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>[6, 14, 6, 26, 26, 68, 146, 226, 366, 1154, 2250, 3884, 8690]</t>
+          <t>[6, 10, 9, 38, 31, 55, 83, 214, 540, 1215, 2008, 4043, 8391]</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 28, 20, 72, 182, 180, 324, 1272, 2376, 4120, 8762]</t>
+          <t>[0, 12, 0, 20, 30, 42, 28, 220, 666, 1282, 1958, 4118, 8606]</t>
         </is>
       </c>
       <c r="J141" t="inlineStr">
@@ -6098,23 +6098,23 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>6.2.d_j_r_bh_bx_da</t>
+          <t>6.2.d_j_r_bh_bx_cy</t>
         </is>
       </c>
       <c r="F142" t="n">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="G142" t="n">
-        <v>53320</v>
+        <v>51480</v>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>[6, 14, 6, 26, 26, 80, 104, 226, 546, 914, 2162, 4364, 8248]</t>
+          <t>[6, 14, 6, 26, 26, 68, 146, 226, 366, 1154, 2250, 3884, 8690]</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 28, 20, 84, 140, 180, 504, 1032, 2288, 4600, 8320]</t>
+          <t>[0, 12, 0, 28, 20, 72, 182, 180, 324, 1272, 2376, 4120, 8762]</t>
         </is>
       </c>
       <c r="J142" t="inlineStr">
@@ -6138,23 +6138,23 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>6.2.d_j_r_bh_bz_dc</t>
+          <t>6.2.d_j_r_bh_bx_da</t>
         </is>
       </c>
       <c r="F143" t="n">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="G143" t="n">
-        <v>50344</v>
+        <v>53320</v>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>[6, 14, 6, 26, 36, 56, 90, 290, 510, 974, 2052, 4316, 8586]</t>
+          <t>[6, 14, 6, 26, 26, 80, 104, 226, 546, 914, 2162, 4364, 8248]</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 28, 30, 60, 126, 244, 468, 1092, 2178, 4552, 8658]</t>
+          <t>[0, 12, 0, 28, 20, 84, 140, 180, 504, 1032, 2288, 4600, 8320]</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -6178,23 +6178,23 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>6.2.d_j_r_bj_cb_di</t>
+          <t>6.2.d_j_r_bh_bz_dc</t>
         </is>
       </c>
       <c r="F144" t="n">
-        <v>890</v>
+        <v>868</v>
       </c>
       <c r="G144" t="n">
-        <v>60520</v>
+        <v>50344</v>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>[6, 14, 6, 34, 16, 56, 132, 210, 582, 1034, 2052, 4108, 8196]</t>
+          <t>[6, 14, 6, 26, 36, 56, 90, 290, 510, 974, 2052, 4316, 8586]</t>
         </is>
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 36, 10, 60, 168, 164, 540, 1152, 2178, 4344, 8268]</t>
+          <t>[0, 12, 0, 28, 30, 60, 126, 244, 468, 1092, 2178, 4552, 8658]</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
@@ -6218,23 +6218,23 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>6.2.d_j_r_bj_cd_dm</t>
+          <t>6.2.d_j_r_bj_cb_di</t>
         </is>
       </c>
       <c r="F145" t="n">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="G145" t="n">
-        <v>59400</v>
+        <v>60520</v>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>[6, 14, 6, 34, 26, 44, 76, 274, 690, 934, 2030, 4156, 7728]</t>
+          <t>[6, 14, 6, 34, 16, 56, 132, 210, 582, 1034, 2052, 4108, 8196]</t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 36, 20, 48, 112, 228, 648, 1052, 2156, 4392, 7800]</t>
+          <t>[0, 12, 0, 36, 10, 60, 168, 164, 540, 1152, 2178, 4344, 8268]</t>
         </is>
       </c>
       <c r="J145" t="inlineStr">
@@ -6258,23 +6258,23 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>6.2.d_j_t_bn_cl_ds</t>
+          <t>6.2.d_j_r_bj_cd_dm</t>
         </is>
       </c>
       <c r="F146" t="n">
-        <v>968</v>
+        <v>900</v>
       </c>
       <c r="G146" t="n">
-        <v>48400</v>
+        <v>59400</v>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>[6, 14, 12, 26, 6, 44, 174, 290, 372, 1154, 2118, 4028, 8430]</t>
+          <t>[6, 14, 6, 34, 26, 44, 76, 274, 690, 934, 2030, 4156, 7728]</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>[0, 12, 6, 28, 0, 48, 210, 244, 330, 1272, 2244, 4264, 8502]</t>
+          <t>[0, 12, 0, 36, 20, 48, 112, 228, 648, 1052, 2156, 4392, 7800]</t>
         </is>
       </c>
       <c r="J146" t="inlineStr">
@@ -6298,28 +6298,28 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>6.2.d_j_t_bn_cl_du</t>
+          <t>6.2.d_j_t_bn_cl_ds</t>
         </is>
       </c>
       <c r="F147" t="n">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="G147" t="n">
-        <v>50440</v>
+        <v>48400</v>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>[6, 14, 12, 26, 6, 56, 132, 290, 516, 1034, 2118, 3884, 8040]</t>
+          <t>[6, 14, 12, 26, 6, 44, 174, 290, 372, 1154, 2118, 4028, 8430]</t>
         </is>
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>[0, 12, 6, 28, 0, 60, 168, 244, 474, 1152, 2244, 4120, 8112]</t>
+          <t>[0, 12, 6, 28, 0, 48, 210, 244, 330, 1272, 2244, 4264, 8502]</t>
         </is>
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6338,28 +6338,28 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>6.2.d_j_t_bn_cl_dw</t>
+          <t>6.2.d_j_t_bn_cl_du</t>
         </is>
       </c>
       <c r="F148" t="n">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="G148" t="n">
-        <v>52488</v>
+        <v>50440</v>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>[6, 14, 12, 26, 6, 68, 90, 290, 660, 914, 2118, 3692, 7962]</t>
+          <t>[6, 14, 12, 26, 6, 56, 132, 290, 516, 1034, 2118, 3884, 8040]</t>
         </is>
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>[0, 12, 6, 28, 0, 72, 126, 244, 618, 1032, 2244, 3928, 8034]</t>
+          <t>[0, 12, 6, 28, 0, 60, 168, 244, 474, 1152, 2244, 4120, 8112]</t>
         </is>
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6371,35 +6371,35 @@
         <v>2</v>
       </c>
       <c r="C149" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D149" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>7.2.d_l_z_cf_dx_gs_js</t>
+          <t>6.2.d_j_t_bn_cl_dw</t>
         </is>
       </c>
       <c r="F149" t="n">
-        <v>2904</v>
+        <v>972</v>
       </c>
       <c r="G149" t="n">
-        <v>435600</v>
+        <v>52488</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>[6, 18, 12, 18, 6, 60, 174, 258, 372, 1218, 2118, 3900, 8430]</t>
+          <t>[6, 14, 12, 26, 6, 68, 90, 290, 660, 914, 2118, 3692, 7962]</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 36, 0, 24, 168, 132, 288, 1332, 2112, 4344, 9048]</t>
+          <t>[0, 12, 6, 28, 0, 72, 126, 244, 618, 1032, 2244, 3928, 8034]</t>
         </is>
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6418,28 +6418,28 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>7.2.d_l_z_cf_dx_gu_js</t>
+          <t>7.2.d_l_z_cf_dx_gs_js</t>
         </is>
       </c>
       <c r="F150" t="n">
-        <v>2910</v>
+        <v>2904</v>
       </c>
       <c r="G150" t="n">
-        <v>453960</v>
+        <v>435600</v>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>[6, 18, 12, 18, 6, 72, 132, 258, 516, 1098, 2118, 3756, 8040]</t>
+          <t>[6, 18, 12, 18, 6, 60, 174, 258, 372, 1218, 2118, 3900, 8430]</t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 36, 0, 36, 126, 132, 432, 1212, 2112, 4200, 8658]</t>
+          <t>[0, 12, 0, 36, 0, 24, 168, 132, 288, 1332, 2112, 4344, 9048]</t>
         </is>
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6458,23 +6458,23 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>7.2.d_l_z_cf_dx_gw_js</t>
+          <t>7.2.d_l_z_cf_dx_gu_js</t>
         </is>
       </c>
       <c r="F151" t="n">
-        <v>2916</v>
+        <v>2910</v>
       </c>
       <c r="G151" t="n">
-        <v>472392</v>
+        <v>453960</v>
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>[6, 18, 12, 18, 6, 84, 90, 258, 660, 978, 2118, 3564, 7962]</t>
+          <t>[6, 18, 12, 18, 6, 72, 132, 258, 516, 1098, 2118, 3756, 8040]</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>[0, 12, 0, 36, 0, 48, 84, 132, 576, 1092, 2112, 4008, 8580]</t>
+          <t>[0, 12, 0, 36, 0, 36, 126, 132, 432, 1212, 2112, 4200, 8658]</t>
         </is>
       </c>
       <c r="J151" t="inlineStr">
@@ -6498,23 +6498,23 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>7.2.e_n_be_cm_ej_hh_ko</t>
+          <t>7.2.d_l_z_cf_dx_gw_js</t>
         </is>
       </c>
       <c r="F152" t="n">
-        <v>3310</v>
+        <v>2916</v>
       </c>
       <c r="G152" t="n">
-        <v>304520</v>
+        <v>472392</v>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>[7, 15, 7, 31, 12, 69, 126, 215, 556, 1040, 2031, 4273, 8236]</t>
+          <t>[6, 18, 12, 18, 6, 84, 90, 258, 660, 978, 2118, 3564, 7962]</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>[0, 14, 0, 30, 0, 38, 84, 126, 576, 1164, 1914, 4314, 8632]</t>
+          <t>[0, 12, 0, 36, 0, 48, 84, 132, 576, 1092, 2112, 4008, 8580]</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
@@ -6538,23 +6538,23 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>7.2.e_n_be_cm_el_hl_kw</t>
+          <t>7.2.e_n_be_cm_ej_hh_ko</t>
         </is>
       </c>
       <c r="F153" t="n">
-        <v>3340</v>
+        <v>3310</v>
       </c>
       <c r="G153" t="n">
-        <v>287240</v>
+        <v>304520</v>
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>[7, 15, 7, 31, 22, 45, 112, 279, 502, 1120, 2119, 3889, 8054]</t>
+          <t>[7, 15, 7, 31, 12, 69, 126, 215, 556, 1040, 2031, 4273, 8236]</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>[0, 14, 0, 30, 10, 14, 70, 190, 522, 1244, 2002, 3930, 8450]</t>
+          <t>[0, 14, 0, 30, 0, 38, 84, 126, 576, 1164, 1914, 4314, 8632]</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
@@ -6578,23 +6578,23 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>7.2.e_n_be_cm_el_hn_ky</t>
+          <t>7.2.e_n_be_cm_el_hl_kw</t>
         </is>
       </c>
       <c r="F154" t="n">
-        <v>3348</v>
+        <v>3340</v>
       </c>
       <c r="G154" t="n">
-        <v>301320</v>
+        <v>287240</v>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>[7, 15, 7, 31, 22, 57, 70, 295, 592, 980, 2339, 3601, 7846]</t>
+          <t>[7, 15, 7, 31, 22, 45, 112, 279, 502, 1120, 2119, 3889, 8054]</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>[0, 14, 0, 30, 10, 26, 28, 206, 612, 1104, 2222, 3642, 8242]</t>
+          <t>[0, 14, 0, 30, 10, 14, 70, 190, 522, 1244, 2002, 3930, 8450]</t>
         </is>
       </c>
       <c r="J154" t="inlineStr">
@@ -6618,23 +6618,23 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>7.2.e_n_be_cm_el_hn_la</t>
+          <t>7.2.e_n_be_cm_el_hn_ky</t>
         </is>
       </c>
       <c r="F155" t="n">
-        <v>3350</v>
+        <v>3348</v>
       </c>
       <c r="G155" t="n">
-        <v>294800</v>
+        <v>301320</v>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>[7, 15, 7, 31, 22, 57, 84, 231, 646, 1180, 1833, 3913, 8366]</t>
+          <t>[7, 15, 7, 31, 22, 57, 70, 295, 592, 980, 2339, 3601, 7846]</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>[0, 14, 0, 30, 10, 26, 42, 142, 666, 1304, 1716, 3954, 8762]</t>
+          <t>[0, 14, 0, 30, 10, 26, 28, 206, 612, 1104, 2222, 3642, 8242]</t>
         </is>
       </c>
       <c r="J155" t="inlineStr">
@@ -6648,38 +6648,38 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C156" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D156" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>2.2.ac_e</t>
+          <t>7.2.e_n_be_cm_el_hn_la</t>
         </is>
       </c>
       <c r="F156" t="n">
-        <v>3</v>
+        <v>3350</v>
       </c>
       <c r="G156" t="n">
-        <v>45</v>
+        <v>294800</v>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>[1, 9, 13, 17, 41, 81, 113, 193, 481, 1089, 2113, 4097, 8321]</t>
+          <t>[7, 15, 7, 31, 22, 57, 84, 231, 646, 1180, 1833, 3913, 8366]</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>[0, 6, 3, 18, 30, 63, 126, 162, 471, 1146, 2046, 4191, 8502]</t>
+          <t>[0, 14, 0, 30, 10, 26, 42, 142, 666, 1304, 1716, 3954, 8762]</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6698,28 +6698,28 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>2.2.a_ab</t>
+          <t>2.2.ac_e</t>
         </is>
       </c>
       <c r="F157" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G157" t="n">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>[3, 3, 9, 31, 33, 87, 129, 223, 513, 903, 2049, 4111, 8193]</t>
+          <t>[1, 9, 13, 17, 41, 81, 113, 193, 481, 1089, 2113, 4097, 8321]</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>[0, 4, 9, 24, 30, 109, 168, 240, 513, 964, 2178, 4125, 7956]</t>
+          <t>[0, 6, 3, 18, 30, 63, 126, 162, 471, 1146, 2046, 4191, 8502]</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6738,23 +6738,23 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>2.2.a_c</t>
+          <t>2.2.a_ab</t>
         </is>
       </c>
       <c r="F158" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G158" t="n">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
+          <t>[3, 3, 9, 31, 33, 87, 129, 223, 513, 903, 2049, 4111, 8193]</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>[0, 10, 9, 18, 30, 55, 168, 306, 513, 1150, 2178, 3855, 7956]</t>
+          <t>[0, 4, 9, 24, 30, 109, 168, 240, 513, 964, 2178, 4125, 7956]</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
@@ -6778,28 +6778,28 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>2.2.b_b</t>
+          <t>2.2.a_c</t>
         </is>
       </c>
       <c r="F159" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G159" t="n">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>[4, 6, 13, 26, 14, 63, 116, 274, 589, 966, 2050, 3935, 8168]</t>
+          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>[0, 6, 21, 42, 30, 63, 84, 210, 525, 966, 2178, 4191, 8424]</t>
+          <t>[0, 10, 9, 18, 30, 55, 168, 306, 513, 1150, 2178, 3855, 7956]</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6818,28 +6818,28 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>2.2.c_c</t>
+          <t>2.2.b_b</t>
         </is>
       </c>
       <c r="F160" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G160" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
+          <t>[4, 6, 13, 26, 14, 63, 116, 274, 589, 966, 2050, 3935, 8168]</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>[1, 5, 25, 25, 41, 65, 113, 225, 385, 1025, 2113, 4609, 8321]</t>
+          <t>[0, 6, 21, 42, 30, 63, 84, 210, 525, 966, 2178, 4191, 8424]</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -6854,32 +6854,32 @@
         <v>2</v>
       </c>
       <c r="D161" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>2.2.a_c</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F161" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G161" t="n">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>[0, 2, 9, 2, 30, 23, 168, 242, 513, 1022, 2178, 3599, 7956]</t>
+          <t>[1, 5, 25, 25, 41, 65, 113, 225, 385, 1025, 2113, 4609, 8321]</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6898,23 +6898,23 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>2.2.a_c</t>
         </is>
       </c>
       <c r="F162" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G162" t="n">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[3, 9, 9, 25, 33, 33, 129, 289, 513, 1089, 2049, 3841, 8193]</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>[0, 2, 12, 26, 0, 56, 126, 290, 516, 902, 1716, 3884, 8190]</t>
+          <t>[0, 2, 9, 2, 30, 23, 168, 242, 513, 1022, 2178, 3599, 7956]</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
@@ -6938,23 +6938,23 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>2.2.b_d</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F163" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G163" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>[0, 2, 12, 14, 30, 44, 189, 302, 534, 1172, 2079, 4136, 8073]</t>
+          <t>[0, 2, 12, 26, 0, 56, 126, 290, 516, 902, 1716, 3884, 8190]</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
@@ -6978,28 +6978,28 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>2.2.c_c</t>
+          <t>2.2.b_d</t>
         </is>
       </c>
       <c r="F164" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G164" t="n">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
+          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>[0, 2, 15, 26, 30, 47, 126, 194, 375, 1082, 2046, 4703, 8502]</t>
+          <t>[0, 2, 12, 14, 30, 44, 189, 302, 534, 1172, 2079, 4136, 8073]</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7011,30 +7011,30 @@
         <v>3</v>
       </c>
       <c r="C165" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D165" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>3.2.ab_c_a</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F165" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G165" t="n">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>[2, 8, 14, 32, 22, 56, 142, 224, 518, 968, 1982, 4400, 8374]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
+          <t>[0, 2, 15, 26, 30, 47, 126, 194, 375, 1082, 2046, 4703, 8502]</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
@@ -7058,28 +7058,28 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>3.2.a_b_a</t>
+          <t>3.2.ab_c_a</t>
         </is>
       </c>
       <c r="F166" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G166" t="n">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>[3, 7, 9, 23, 33, 103, 129, 191, 513, 967, 2049, 3983, 8193]</t>
+          <t>[2, 8, 14, 32, 22, 56, 142, 224, 518, 968, 1982, 4400, 8374]</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>[0, 0, 9, 0, 30, 93, 168, 144, 513, 900, 2178, 3741, 7956]</t>
+          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
         </is>
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7098,23 +7098,23 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>3.2.a_b_d</t>
+          <t>3.2.a_b_a</t>
         </is>
       </c>
       <c r="F167" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G167" t="n">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>[3, 7, 18, 23, 18, 76, 108, 263, 459, 1012, 2247, 4172, 8310]</t>
+          <t>[3, 7, 9, 23, 33, 103, 129, 191, 513, 967, 2049, 3983, 8193]</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>[0, 0, 18, 0, 15, 66, 147, 216, 459, 945, 2376, 3930, 8073]</t>
+          <t>[0, 0, 9, 0, 30, 93, 168, 144, 513, 900, 2178, 3741, 7956]</t>
         </is>
       </c>
       <c r="J167" t="inlineStr">
@@ -7138,23 +7138,23 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>3.2.b_b_b</t>
+          <t>3.2.a_b_d</t>
         </is>
       </c>
       <c r="F168" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G168" t="n">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>[4, 6, 10, 22, 44, 90, 74, 254, 496, 966, 2050, 4198, 8636]</t>
+          <t>[3, 7, 18, 23, 18, 76, 108, 263, 459, 1012, 2247, 4172, 8310]</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 24, 30, 90, 42, 288, 462, 900, 1848, 3810, 8580]</t>
+          <t>[0, 0, 18, 0, 15, 66, 147, 216, 459, 945, 2376, 3930, 8073]</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
@@ -7178,23 +7178,23 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>3.2.b_b_e</t>
+          <t>3.2.b_b_b</t>
         </is>
       </c>
       <c r="F169" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G169" t="n">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>[4, 6, 19, 10, 44, 63, 116, 194, 523, 1146, 2116, 4063, 8012]</t>
+          <t>[4, 6, 10, 22, 44, 90, 74, 254, 496, 966, 2050, 4198, 8636]</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>[0, 0, 21, 12, 30, 63, 84, 228, 489, 1080, 1914, 3675, 7956]</t>
+          <t>[0, 0, 12, 24, 30, 90, 42, 288, 462, 900, 1848, 3810, 8580]</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
@@ -7218,28 +7218,28 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>3.2.b_c_a</t>
+          <t>3.2.b_b_e</t>
         </is>
       </c>
       <c r="F170" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G170" t="n">
-        <v>200</v>
+        <v>63</v>
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>[4, 8, 4, 32, 44, 56, 116, 224, 508, 968, 2116, 4400, 8012]</t>
+          <t>[4, 6, 19, 10, 44, 63, 116, 194, 523, 1146, 2116, 4063, 8012]</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 32, 60, 24, 84, 96, 444, 840, 2244, 4400, 8268]</t>
+          <t>[0, 0, 21, 12, 30, 63, 84, 228, 489, 1080, 1914, 3675, 7956]</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7258,28 +7258,28 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>3.2.b_c_b</t>
+          <t>3.2.b_c_a</t>
         </is>
       </c>
       <c r="F171" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G171" t="n">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>[4, 8, 7, 28, 39, 71, 88, 220, 574, 943, 2138, 4375, 8051]</t>
+          <t>[4, 8, 4, 32, 44, 56, 116, 224, 508, 968, 2116, 4400, 8012]</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 24, 45, 60, 105, 264, 669, 1065, 2145, 4368, 7800]</t>
+          <t>[0, 0, 12, 32, 60, 24, 84, 96, 444, 840, 2244, 4400, 8268]</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7298,28 +7298,28 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>3.2.b_c_d</t>
+          <t>3.2.b_c_b</t>
         </is>
       </c>
       <c r="F172" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G172" t="n">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>[4, 8, 13, 20, 29, 83, 74, 236, 562, 1103, 2116, 3887, 8363]</t>
+          <t>[4, 8, 7, 28, 39, 71, 88, 220, 574, 943, 2138, 4375, 8051]</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>[0, 0, 21, 20, 45, 51, 42, 108, 498, 975, 2244, 3887, 8619]</t>
+          <t>[0, 0, 12, 24, 45, 60, 105, 264, 669, 1065, 2145, 4368, 7800]</t>
         </is>
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7354,7 +7354,7 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>[0, 2, 15, 22, 15, 83, 42, 270, 528, 1037, 1914, 3499, 8307]</t>
+          <t>[0, 0, 21, 20, 45, 51, 42, 108, 498, 975, 2244, 3887, 8619]</t>
         </is>
       </c>
       <c r="J173" t="inlineStr">
@@ -7378,28 +7378,28 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>3.2.b_c_e</t>
+          <t>3.2.b_c_d</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G174" t="n">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>[4, 8, 16, 16, 24, 80, 88, 256, 520, 1168, 2072, 3808, 8168]</t>
+          <t>[4, 8, 13, 20, 29, 83, 74, 236, 562, 1103, 2116, 3887, 8363]</t>
         </is>
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>[0, 0, 21, 12, 30, 69, 105, 300, 615, 1290, 2079, 3801, 7917]</t>
+          <t>[0, 2, 15, 22, 15, 83, 42, 270, 528, 1037, 1914, 3499, 8307]</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7418,28 +7418,28 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>3.2.b_d_e</t>
+          <t>3.2.b_c_e</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G175" t="n">
-        <v>243</v>
+        <v>144</v>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>[4, 10, 13, 18, 14, 79, 116, 242, 589, 1030, 2050, 3807, 8168]</t>
+          <t>[4, 8, 16, 16, 24, 80, 88, 256, 520, 1168, 2072, 3808, 8168]</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>[0, 2, 21, 18, 30, 47, 84, 114, 525, 902, 2178, 3807, 8424]</t>
+          <t>[0, 0, 21, 12, 30, 69, 105, 300, 615, 1290, 2079, 3801, 7917]</t>
         </is>
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7458,28 +7458,28 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>3.2.b_e_e</t>
+          <t>3.2.b_d_e</t>
         </is>
       </c>
       <c r="F176" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G176" t="n">
-        <v>360</v>
+        <v>243</v>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>[4, 12, 10, 16, 14, 72, 158, 224, 550, 1032, 1918, 4144, 8246]</t>
+          <t>[4, 10, 13, 18, 14, 79, 116, 242, 589, 1030, 2050, 3807, 8168]</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>[0, 6, 12, 18, 0, 72, 126, 258, 516, 966, 1716, 3756, 8190]</t>
+          <t>[0, 2, 21, 18, 30, 47, 84, 114, 525, 902, 2178, 3807, 8424]</t>
         </is>
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7498,28 +7498,28 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>3.2.c_d_f</t>
+          <t>3.2.b_e_e</t>
         </is>
       </c>
       <c r="F177" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G177" t="n">
-        <v>99</v>
+        <v>360</v>
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>[5, 7, 14, 15, 40, 52, 82, 311, 545, 1072, 1919, 4212, 7870]</t>
+          <t>[4, 12, 10, 16, 14, 72, 158, 224, 550, 1032, 1918, 4144, 8246]</t>
         </is>
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>[1, 1, 16, 17, 26, 52, 50, 345, 511, 1006, 1717, 3824, 7814]</t>
+          <t>[0, 6, 12, 18, 0, 72, 126, 258, 516, 966, 1716, 3756, 8190]</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7538,23 +7538,23 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>3.2.c_e_h</t>
+          <t>3.2.c_d_f</t>
         </is>
       </c>
       <c r="F178" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G178" t="n">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>[5, 9, 14, 9, 25, 78, 103, 305, 518, 1029, 1853, 4158, 8611]</t>
+          <t>[5, 7, 14, 15, 40, 52, 82, 311, 545, 1072, 1919, 4212, 7870]</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>[1, 1, 22, 9, 41, 46, 71, 177, 454, 901, 1981, 4158, 8867]</t>
+          <t>[1, 1, 16, 17, 26, 52, 50, 345, 511, 1006, 1717, 3824, 7814]</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
@@ -7594,7 +7594,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>[1, 3, 16, 11, 11, 78, 71, 339, 484, 963, 1651, 3770, 8555]</t>
+          <t>[1, 1, 22, 9, 41, 46, 71, 177, 454, 901, 1981, 4158, 8867]</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
@@ -7618,23 +7618,23 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>3.2.d_h_l</t>
+          <t>3.2.c_e_h</t>
         </is>
       </c>
       <c r="F180" t="n">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="G180" t="n">
-        <v>224</v>
+        <v>152</v>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>[6, 10, 6, 14, 26, 82, 118, 286, 474, 930, 2294, 4046, 7962]</t>
+          <t>[5, 9, 14, 9, 25, 78, 103, 305, 518, 1029, 1853, 4158, 8611]</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>[2, 2, 14, 14, 42, 50, 86, 158, 410, 802, 2422, 4046, 8218]</t>
+          <t>[1, 3, 16, 11, 11, 78, 71, 339, 484, 963, 1651, 3770, 8555]</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
@@ -7651,30 +7651,30 @@
         <v>3</v>
       </c>
       <c r="C181" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D181" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>4.2.d_f_i_n</t>
+          <t>3.2.d_h_l</t>
         </is>
       </c>
       <c r="F181" t="n">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="G181" t="n">
-        <v>424</v>
+        <v>224</v>
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>[6, 6, 15, 22, 21, 87, 97, 214, 510, 1151, 2118, 4123, 7793]</t>
+          <t>[6, 10, 6, 14, 26, 82, 118, 286, 474, 930, 2294, 4046, 7962]</t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>[0, 0, 18, 4, 20, 42, 42, 92, 540, 1090, 2068, 3814, 8008]</t>
+          <t>[2, 2, 14, 14, 42, 50, 86, 158, 410, 802, 2422, 4046, 8218]</t>
         </is>
       </c>
       <c r="J181" t="inlineStr">
@@ -7698,28 +7698,28 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>4.2.d_f_k_s</t>
+          <t>4.2.d_f_i_n</t>
         </is>
       </c>
       <c r="F182" t="n">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="G182" t="n">
-        <v>351</v>
+        <v>424</v>
       </c>
       <c r="H182" t="inlineStr">
         <is>
-          <t>[6, 6, 21, 18, 6, 63, 132, 306, 525, 966, 1986, 4191, 8040]</t>
+          <t>[6, 6, 15, 22, 21, 87, 97, 214, 510, 1151, 2118, 4123, 7793]</t>
         </is>
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>[0, 0, 18, 0, 0, 72, 126, 360, 549, 990, 1683, 4212, 8073]</t>
+          <t>[0, 0, 18, 4, 20, 42, 42, 92, 540, 1090, 2068, 3814, 8008]</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7738,23 +7738,23 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>4.2.e_j_q_z</t>
+          <t>4.2.d_f_k_s</t>
         </is>
       </c>
       <c r="F183" t="n">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="G183" t="n">
-        <v>513</v>
+        <v>351</v>
       </c>
       <c r="H183" t="inlineStr">
         <is>
-          <t>[7, 7, 13, 19, 17, 85, 77, 291, 589, 1027, 1921, 3949, 8405]</t>
+          <t>[6, 6, 21, 18, 6, 63, 132, 306, 525, 966, 1986, 4191, 8040]</t>
         </is>
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>[0, 0, 21, 12, 30, 75, 84, 180, 525, 960, 2178, 3963, 8424]</t>
+          <t>[0, 0, 18, 0, 0, 72, 126, 360, 549, 990, 1683, 4212, 8073]</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
@@ -7778,28 +7778,28 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>4.2.e_k_u_bg</t>
+          <t>4.2.e_j_q_z</t>
         </is>
       </c>
       <c r="F184" t="n">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="G184" t="n">
-        <v>585</v>
+        <v>513</v>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>[7, 9, 13, 9, 17, 81, 161, 225, 481, 1089, 1921, 4353, 7937]</t>
+          <t>[7, 7, 13, 19, 17, 85, 77, 291, 589, 1027, 1921, 3949, 8405]</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>[0, 2, 21, 2, 30, 71, 168, 114, 417, 1022, 2178, 4367, 7956]</t>
+          <t>[0, 0, 21, 12, 30, 75, 84, 180, 525, 960, 2178, 3963, 8424]</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7818,23 +7818,23 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>4.2.f_o_bc_bs</t>
+          <t>4.2.e_k_u_bg</t>
         </is>
       </c>
       <c r="F185" t="n">
-        <v>260</v>
+        <v>195</v>
       </c>
       <c r="G185" t="n">
-        <v>520</v>
+        <v>585</v>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>[8, 8, 8, 16, 28, 56, 148, 288, 476, 968, 1988, 4528, 7756]</t>
+          <t>[7, 9, 13, 9, 17, 81, 161, 225, 481, 1089, 1921, 4353, 7937]</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>[0, 0, 24, 32, 60, 24, 84, 96, 348, 840, 2244, 4784, 8268]</t>
+          <t>[0, 2, 21, 2, 30, 71, 168, 114, 417, 1022, 2178, 4367, 7956]</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
@@ -7848,38 +7848,38 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
+        <v>3</v>
+      </c>
+      <c r="C186" t="n">
         <v>4</v>
       </c>
-      <c r="C186" t="n">
-        <v>2</v>
-      </c>
       <c r="D186" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>2.2.ab_c</t>
+          <t>4.2.f_o_bc_bs</t>
         </is>
       </c>
       <c r="F186" t="n">
-        <v>4</v>
+        <v>260</v>
       </c>
       <c r="G186" t="n">
-        <v>40</v>
+        <v>520</v>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>[2, 8, 8, 24, 52, 56, 100, 256, 476, 968, 2180, 4272, 8140]</t>
+          <t>[8, 8, 8, 16, 28, 56, 148, 288, 476, 968, 1988, 4528, 7756]</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 16, 60, 24, 84, 160, 444, 840, 2244, 4144, 8268]</t>
+          <t>[0, 0, 24, 32, 60, 24, 84, 96, 348, 840, 2244, 4784, 8268]</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7898,28 +7898,28 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>2.2.b_a</t>
+          <t>2.2.ab_c</t>
         </is>
       </c>
       <c r="F187" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G187" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>[4, 4, 16, 24, 24, 64, 88, 288, 520, 1104, 2072, 3936, 8168]</t>
+          <t>[2, 8, 8, 24, 52, 56, 100, 256, 476, 968, 2180, 4272, 8140]</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>[0, 4, 12, 24, 40, 64, 56, 288, 552, 1104, 2200, 4320, 8424]</t>
+          <t>[0, 0, 12, 16, 60, 24, 84, 160, 444, 840, 2244, 4144, 8268]</t>
         </is>
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -7938,23 +7938,23 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>2.2.b_a</t>
         </is>
       </c>
       <c r="F188" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G188" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[4, 4, 16, 24, 24, 64, 88, 288, 520, 1104, 2072, 3936, 8168]</t>
         </is>
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>[0, 8, 6, 24, 30, 56, 126, 256, 582, 968, 2046, 4656, 8502]</t>
+          <t>[0, 4, 12, 24, 40, 64, 56, 288, 552, 1104, 2200, 4320, 8424]</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
@@ -7978,23 +7978,23 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F189" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G189" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>[1, 9, 1, 17, 41, 81, 113, 193, 577, 1089, 2113, 4481, 8321]</t>
+          <t>[0, 8, 6, 24, 30, 56, 126, 256, 582, 968, 2046, 4656, 8502]</t>
         </is>
       </c>
       <c r="J189" t="inlineStr">
@@ -8014,7 +8014,7 @@
         <v>2</v>
       </c>
       <c r="D190" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -8034,7 +8034,7 @@
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>[1, 1, 13, 17, 41, 49, 113, 65, 481, 961, 2113, 4097, 8321]</t>
+          <t>[1, 9, 1, 17, 41, 81, 113, 193, 577, 1089, 2113, 4481, 8321]</t>
         </is>
       </c>
       <c r="J190" t="inlineStr">
@@ -8051,30 +8051,30 @@
         <v>4</v>
       </c>
       <c r="C191" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D191" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>3.2.c_e_f</t>
+          <t>2.2.c_e</t>
         </is>
       </c>
       <c r="F191" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="G191" t="n">
-        <v>216</v>
+        <v>45</v>
       </c>
       <c r="H191" t="inlineStr">
         <is>
-          <t>[5, 9, 8, 25, 25, 54, 103, 305, 584, 909, 2117, 3982, 7987]</t>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
         </is>
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 28, 0, 36, 84, 308, 540, 900, 1848, 3688, 8112]</t>
+          <t>[1, 1, 13, 17, 41, 49, 113, 65, 481, 961, 2113, 4097, 8321]</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
@@ -8098,23 +8098,23 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>3.2.d_g_i</t>
+          <t>3.2.c_e_f</t>
         </is>
       </c>
       <c r="F192" t="n">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="G192" t="n">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>[6, 8, 6, 32, 6, 56, 174, 224, 582, 968, 1854, 4400, 8118]</t>
+          <t>[5, 9, 8, 25, 25, 54, 103, 305, 584, 909, 2117, 3982, 7987]</t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>[0, 0, 6, 24, 30, 24, 126, 128, 582, 840, 2046, 4656, 8502]</t>
+          <t>[0, 0, 0, 28, 0, 36, 84, 308, 540, 900, 1848, 3688, 8112]</t>
         </is>
       </c>
       <c r="J192" t="inlineStr">
@@ -8128,38 +8128,38 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C193" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D193" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>2.2.a_a</t>
+          <t>3.2.d_g_i</t>
         </is>
       </c>
       <c r="F193" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G193" t="n">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="H193" t="inlineStr">
         <is>
-          <t>[3, 5, 9, 33, 33, 65, 129, 193, 513, 1025, 2049, 4353, 8193]</t>
+          <t>[6, 8, 6, 32, 6, 56, 174, 224, 582, 968, 1854, 4400, 8118]</t>
         </is>
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 20, 15, 90, 105, 180, 540, 1075, 2145, 4130, 8385]</t>
+          <t>[0, 0, 6, 24, 30, 24, 126, 128, 582, 840, 2046, 4656, 8502]</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8178,28 +8178,28 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>2.2.a_b</t>
+          <t>2.2.a_a</t>
         </is>
       </c>
       <c r="F194" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G194" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>[3, 7, 9, 31, 33, 43, 129, 223, 513, 1147, 2049, 4111, 8193]</t>
+          <t>[3, 5, 9, 33, 33, 65, 129, 193, 513, 1025, 2049, 4353, 8193]</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>[0, 0, 9, 8, 30, 33, 168, 176, 513, 1080, 2178, 3869, 7956]</t>
+          <t>[0, 0, 0, 20, 15, 90, 105, 180, 540, 1075, 2145, 4130, 8385]</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8218,28 +8218,28 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>2.2.a_b</t>
         </is>
       </c>
       <c r="F195" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G195" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[3, 7, 9, 31, 33, 43, 129, 223, 513, 1147, 2049, 4111, 8193]</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>[0, 0, 15, 20, 20, 45, 175, 300, 645, 1090, 1925, 4265, 7995]</t>
+          <t>[0, 0, 9, 8, 30, 33, 168, 176, 513, 1080, 2178, 3869, 7956]</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8274,12 +8274,12 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>[0, 6, 0, 18, 0, 60, 210, 242, 540, 1086, 1980, 4380, 8190]</t>
+          <t>[0, 0, 15, 20, 20, 45, 175, 300, 645, 1090, 1925, 4265, 7995]</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8298,23 +8298,23 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>2.2.b_d</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F197" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G197" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>[0, 2, 15, 18, 40, 23, 140, 130, 375, 922, 2200, 4143, 8580]</t>
+          <t>[0, 6, 0, 18, 0, 60, 210, 242, 540, 1086, 1980, 4380, 8190]</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
@@ -8338,23 +8338,23 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>2.2.b_d</t>
         </is>
       </c>
       <c r="F198" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G198" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[4, 10, 7, 18, 24, 55, 172, 258, 439, 1050, 2072, 4143, 8324]</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>[0, 6, 3, 34, 30, 63, 126, 98, 471, 1146, 2046, 4447, 8502]</t>
+          <t>[0, 2, 15, 18, 40, 23, 140, 130, 375, 922, 2200, 4143, 8580]</t>
         </is>
       </c>
       <c r="J198" t="inlineStr">
@@ -8394,12 +8394,12 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>[0, 10, 0, 10, 25, 70, 140, 210, 450, 845, 1870, 4090, 7800]</t>
+          <t>[0, 6, 3, 34, 30, 63, 126, 98, 471, 1146, 2046, 4447, 8502]</t>
         </is>
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -8418,28 +8418,28 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>2.2.d_f</t>
+          <t>2.2.c_e</t>
         </is>
       </c>
       <c r="F200" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G200" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>[1, 3, 7, 27, 41, 69, 71, 179, 439, 1143, 1981, 4461, 8867]</t>
+          <t>[0, 10, 0, 10, 25, 70, 140, 210, 450, 845, 1870, 4090, 7800]</t>
         </is>
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8448,33 +8448,33 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
+        <v>5</v>
+      </c>
+      <c r="C201" t="n">
+        <v>2</v>
+      </c>
+      <c r="D201" t="n">
         <v>6</v>
       </c>
-      <c r="C201" t="n">
-        <v>2</v>
-      </c>
-      <c r="D201" t="n">
-        <v>7</v>
-      </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>2.2.b_c</t>
+          <t>2.2.d_f</t>
         </is>
       </c>
       <c r="F201" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G201" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
         </is>
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
+          <t>[1, 3, 7, 27, 41, 69, 71, 179, 439, 1143, 1981, 4461, 8867]</t>
         </is>
       </c>
       <c r="J201" t="inlineStr">
@@ -8498,23 +8498,23 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>2.2.c_c</t>
+          <t>2.2.b_c</t>
         </is>
       </c>
       <c r="F202" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G202" t="n">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
+          <t>[4, 8, 10, 24, 14, 56, 158, 256, 550, 968, 1918, 4272, 8246]</t>
         </is>
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>[0, 0, 12, 4, 15, 90, 105, 244, 444, 1075, 2145, 4258, 8385]</t>
+          <t>[0, 0, 6, 8, 30, 24, 126, 192, 582, 840, 2046, 4400, 8502]</t>
         </is>
       </c>
       <c r="J202" t="inlineStr">
@@ -8554,7 +8554,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>[0, 2, 3, 10, 30, 47, 126, 258, 471, 1082, 2046, 4831, 8502]</t>
+          <t>[0, 0, 12, 4, 15, 90, 105, 244, 444, 1075, 2145, 4258, 8385]</t>
         </is>
       </c>
       <c r="J203" t="inlineStr">
@@ -8578,23 +8578,23 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>2.2.c_d</t>
+          <t>2.2.c_c</t>
         </is>
       </c>
       <c r="F204" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G204" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H204" t="inlineStr">
         <is>
-          <t>[5, 7, 11, 15, 15, 91, 131, 255, 479, 987, 2227, 3999, 8143]</t>
+          <t>[5, 5, 17, 9, 25, 65, 145, 289, 449, 1025, 1985, 4353, 8065]</t>
         </is>
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>[0, 2, 6, 10, 5, 116, 91, 210, 474, 1037, 2387, 3904, 8463]</t>
+          <t>[0, 2, 3, 10, 30, 47, 126, 258, 471, 1082, 2046, 4831, 8502]</t>
         </is>
       </c>
       <c r="J204" t="inlineStr">
@@ -8618,23 +8618,23 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>2.2.c_e</t>
+          <t>2.2.c_d</t>
         </is>
       </c>
       <c r="F205" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G205" t="n">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
+          <t>[5, 7, 11, 15, 15, 91, 131, 255, 479, 987, 2227, 3999, 8143]</t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>[1, 1, 1, 1, 41, 49, 113, 129, 577, 961, 2113, 4225, 8321]</t>
+          <t>[0, 2, 6, 10, 5, 116, 91, 210, 474, 1037, 2387, 3904, 8463]</t>
         </is>
       </c>
       <c r="J205" t="inlineStr">
@@ -8658,23 +8658,23 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>2.2.d_f</t>
+          <t>2.2.c_e</t>
         </is>
       </c>
       <c r="F206" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G206" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+          <t>[5, 9, 5, 17, 25, 81, 145, 193, 545, 1089, 1985, 4097, 8065]</t>
         </is>
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>[0, 2, 3, 14, 35, 131, 168, 286, 570, 1137, 2002, 4259, 8099]</t>
+          <t>[1, 1, 1, 1, 41, 49, 113, 129, 577, 961, 2113, 4225, 8321]</t>
         </is>
       </c>
       <c r="J206" t="inlineStr">
@@ -8714,7 +8714,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>[0, 4, 3, 12, 30, 91, 126, 228, 471, 1204, 2046, 4347, 8502]</t>
+          <t>[0, 2, 3, 14, 35, 131, 168, 286, 570, 1137, 2002, 4259, 8099]</t>
         </is>
       </c>
       <c r="J207" t="inlineStr">
@@ -8728,36 +8728,76 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
+        <v>6</v>
+      </c>
+      <c r="C208" t="n">
+        <v>2</v>
+      </c>
+      <c r="D208" t="n">
         <v>7</v>
       </c>
-      <c r="C208" t="n">
-        <v>2</v>
-      </c>
-      <c r="D208" t="n">
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>2.2.d_f</t>
+        </is>
+      </c>
+      <c r="F208" t="n">
+        <v>19</v>
+      </c>
+      <c r="G208" t="n">
+        <v>19</v>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>[6, 6, 9, 10, 36, 87, 90, 274, 513, 1086, 1920, 4111, 8430]</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>[0, 4, 3, 12, 30, 91, 126, 228, 471, 1204, 2046, 4347, 8502]</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>7</v>
+      </c>
+      <c r="C209" t="n">
+        <v>2</v>
+      </c>
+      <c r="D209" t="n">
         <v>8</v>
       </c>
-      <c r="E208" t="inlineStr">
+      <c r="E209" t="inlineStr">
         <is>
           <t>2.2.c_d</t>
         </is>
       </c>
-      <c r="F208" t="n">
+      <c r="F209" t="n">
         <v>14</v>
       </c>
-      <c r="G208" t="n">
+      <c r="G209" t="n">
         <v>28</v>
       </c>
-      <c r="H208" t="inlineStr">
+      <c r="H209" t="inlineStr">
         <is>
           <t>[5, 7, 11, 15, 15, 91, 131, 255, 479, 987, 2227, 3999, 8143]</t>
         </is>
       </c>
-      <c r="I208" t="inlineStr">
+      <c r="I209" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 84, 133, 336, 378, 980, 2310, 4032, 8008]</t>
         </is>
       </c>
-      <c r="J208" t="inlineStr">
+      <c r="J209" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>